<commit_message>
added networks 30 & 31
</commit_message>
<xml_diff>
--- a/data/15-gene_networks_analysis/pvalue_MSE_comparison.xlsx
+++ b/data/15-gene_networks_analysis/pvalue_MSE_comparison.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" tabRatio="717" firstSheet="3" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" tabRatio="717" firstSheet="2" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="wt" sheetId="1" r:id="rId1"/>
@@ -62,7 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1556" uniqueCount="174">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1634" uniqueCount="176">
   <si>
     <t>Gene</t>
   </si>
@@ -585,6 +585,12 @@
   <si>
     <t>rand31</t>
   </si>
+  <si>
+    <t>Difference between random network 30 and db network 5 individual MSE values</t>
+  </si>
+  <si>
+    <t>Difference between random network 31 and db network 5 individual MSE values</t>
+  </si>
 </sst>
 </file>
 
@@ -899,9 +905,9 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>dhap4!$U$2:$U$31</c:f>
+              <c:f>dhap4!$U$2:$U$33</c:f>
               <c:strCache>
-                <c:ptCount val="30"/>
+                <c:ptCount val="32"/>
                 <c:pt idx="0">
                   <c:v>db5</c:v>
                 </c:pt>
@@ -992,15 +998,21 @@
                 <c:pt idx="29">
                   <c:v>rand29</c:v>
                 </c:pt>
+                <c:pt idx="30">
+                  <c:v>rand30</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>rand31</c:v>
+                </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>dhap4!$V$2:$V$31</c:f>
+              <c:f>dhap4!$V$2:$V$33</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="30"/>
+                <c:ptCount val="32"/>
                 <c:pt idx="0">
                   <c:v>1.4262899447569053</c:v>
                 </c:pt>
@@ -1091,6 +1103,12 @@
                 <c:pt idx="29">
                   <c:v>1.4434426448330233</c:v>
                 </c:pt>
+                <c:pt idx="30">
+                  <c:v>1.4760844231147061</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>1.5009483703776725</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -1118,9 +1136,9 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>dhap4!$U$2:$U$31</c:f>
+              <c:f>dhap4!$U$2:$U$33</c:f>
               <c:strCache>
-                <c:ptCount val="30"/>
+                <c:ptCount val="32"/>
                 <c:pt idx="0">
                   <c:v>db5</c:v>
                 </c:pt>
@@ -1211,6 +1229,12 @@
                 <c:pt idx="29">
                   <c:v>rand29</c:v>
                 </c:pt>
+                <c:pt idx="30">
+                  <c:v>rand30</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>rand31</c:v>
+                </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
@@ -1247,9 +1271,9 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>dhap4!$U$2:$U$31</c:f>
+              <c:f>dhap4!$U$2:$U$33</c:f>
               <c:strCache>
-                <c:ptCount val="30"/>
+                <c:ptCount val="32"/>
                 <c:pt idx="0">
                   <c:v>db5</c:v>
                 </c:pt>
@@ -1340,6 +1364,12 @@
                 <c:pt idx="29">
                   <c:v>rand29</c:v>
                 </c:pt>
+                <c:pt idx="30">
+                  <c:v>rand30</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>rand31</c:v>
+                </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
@@ -1362,8 +1392,8 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="219"/>
-        <c:axId val="159840480"/>
-        <c:axId val="159841040"/>
+        <c:axId val="89194320"/>
+        <c:axId val="277034832"/>
       </c:barChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -1385,9 +1415,9 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>dhap4!$U$2:$U$31</c:f>
+              <c:f>dhap4!$U$2:$U$33</c:f>
               <c:strCache>
-                <c:ptCount val="30"/>
+                <c:ptCount val="32"/>
                 <c:pt idx="0">
                   <c:v>db5</c:v>
                 </c:pt>
@@ -1478,15 +1508,21 @@
                 <c:pt idx="29">
                   <c:v>rand29</c:v>
                 </c:pt>
+                <c:pt idx="30">
+                  <c:v>rand30</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>rand31</c:v>
+                </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>dhap4!$W$2:$W$31</c:f>
+              <c:f>dhap4!$W$2:$W$33</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="30"/>
+                <c:ptCount val="32"/>
                 <c:pt idx="0">
                   <c:v>1.4262899447569053</c:v>
                 </c:pt>
@@ -1577,6 +1613,12 @@
                 <c:pt idx="29">
                   <c:v>1.42628994475691</c:v>
                 </c:pt>
+                <c:pt idx="30">
+                  <c:v>1.42628994475691</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>1.42628994475691</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -1592,11 +1634,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="159840480"/>
-        <c:axId val="159841040"/>
+        <c:axId val="89194320"/>
+        <c:axId val="277034832"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="159840480"/>
+        <c:axId val="89194320"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1639,7 +1681,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="159841040"/>
+        <c:crossAx val="277034832"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1647,7 +1689,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="159841040"/>
+        <c:axId val="277034832"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1.5249999999999999"/>
@@ -1700,7 +1742,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="159840480"/>
+        <c:crossAx val="89194320"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2296,16 +2338,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>24</xdr:col>
-      <xdr:colOff>395287</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>176212</xdr:rowOff>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>366711</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>33336</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>32</xdr:col>
-      <xdr:colOff>242887</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>23812</xdr:rowOff>
+      <xdr:col>36</xdr:col>
+      <xdr:colOff>333374</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>266699</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3491,6 +3533,12 @@
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="P7:U7"/>
+    <mergeCell ref="P2:U2"/>
+    <mergeCell ref="P4:U4"/>
+    <mergeCell ref="P3:U3"/>
+    <mergeCell ref="P5:U5"/>
+    <mergeCell ref="P6:U6"/>
     <mergeCell ref="P14:U14"/>
     <mergeCell ref="P15:U15"/>
     <mergeCell ref="P16:U16"/>
@@ -3501,12 +3549,6 @@
     <mergeCell ref="P11:U11"/>
     <mergeCell ref="P12:U12"/>
     <mergeCell ref="P13:U13"/>
-    <mergeCell ref="P7:U7"/>
-    <mergeCell ref="P2:U2"/>
-    <mergeCell ref="P4:U4"/>
-    <mergeCell ref="P3:U3"/>
-    <mergeCell ref="P5:U5"/>
-    <mergeCell ref="P6:U6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200"/>
@@ -15618,11 +15660,6 @@
     </row>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="N14:S14"/>
-    <mergeCell ref="N15:S15"/>
-    <mergeCell ref="N16:S16"/>
-    <mergeCell ref="N17:S17"/>
-    <mergeCell ref="N18:S18"/>
     <mergeCell ref="N13:S13"/>
     <mergeCell ref="N2:S2"/>
     <mergeCell ref="N3:S3"/>
@@ -15635,6 +15672,11 @@
     <mergeCell ref="N10:S10"/>
     <mergeCell ref="N11:S11"/>
     <mergeCell ref="N12:S12"/>
+    <mergeCell ref="N14:S14"/>
+    <mergeCell ref="N15:S15"/>
+    <mergeCell ref="N16:S16"/>
+    <mergeCell ref="N17:S17"/>
+    <mergeCell ref="N18:S18"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -31975,6 +32017,1127 @@
   <dimension ref="A1:M38"/>
   <sheetViews>
     <sheetView workbookViewId="0">
+      <selection activeCell="A20" sqref="A20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="F1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="H1" t="s">
+        <v>4</v>
+      </c>
+      <c r="I1" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="J1" t="s">
+        <v>5</v>
+      </c>
+      <c r="K1" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="L1" t="s">
+        <v>6</v>
+      </c>
+      <c r="M1" s="19" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2">
+        <v>0.51820630315546445</v>
+      </c>
+      <c r="C2" s="14">
+        <v>0.762384490029694</v>
+      </c>
+      <c r="D2">
+        <v>0.15342967430076551</v>
+      </c>
+      <c r="E2" s="15">
+        <v>0.44624975588118598</v>
+      </c>
+      <c r="F2">
+        <v>1.3375201575909201</v>
+      </c>
+      <c r="G2" s="16">
+        <v>0.78551996118716705</v>
+      </c>
+      <c r="H2">
+        <v>0.10769502062634854</v>
+      </c>
+      <c r="I2" s="17">
+        <v>0.29160072506103601</v>
+      </c>
+      <c r="J2">
+        <v>0.21526229159377588</v>
+      </c>
+      <c r="K2" s="18">
+        <v>0.82577386681059695</v>
+      </c>
+      <c r="L2">
+        <v>1.0159260346188708</v>
+      </c>
+      <c r="M2" s="7">
+        <v>4.5710095337786E-2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3">
+        <v>0.30180799437297201</v>
+      </c>
+      <c r="C3" s="14">
+        <v>8.2901279432195593E-2</v>
+      </c>
+      <c r="D3">
+        <v>0.78961568801773474</v>
+      </c>
+      <c r="E3" s="9">
+        <v>9.0782211164155292E-3</v>
+      </c>
+      <c r="F3">
+        <v>0.54591947676929864</v>
+      </c>
+      <c r="G3" s="16">
+        <v>0.52024738694317496</v>
+      </c>
+      <c r="H3">
+        <v>0.38238981323261939</v>
+      </c>
+      <c r="I3" s="17">
+        <v>7.2269282640789106E-2</v>
+      </c>
+      <c r="J3">
+        <v>1.1943672882960155</v>
+      </c>
+      <c r="K3" s="18">
+        <v>0.76388269721491497</v>
+      </c>
+      <c r="L3">
+        <v>1.2454099030617656</v>
+      </c>
+      <c r="M3" s="19">
+        <v>0.45347930983877699</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4">
+        <v>0.60003795339805421</v>
+      </c>
+      <c r="C4" s="14">
+        <v>6.6225124959576706E-2</v>
+      </c>
+      <c r="D4">
+        <v>0.14496421249999999</v>
+      </c>
+      <c r="E4" s="15">
+        <v>0.61881514010194805</v>
+      </c>
+      <c r="F4">
+        <v>1.1803841392068706</v>
+      </c>
+      <c r="G4" s="10">
+        <v>1.6347989883004101E-2</v>
+      </c>
+      <c r="H4">
+        <v>0.93850425171750873</v>
+      </c>
+      <c r="I4" s="11">
+        <v>1.1178235493982801E-2</v>
+      </c>
+      <c r="J4">
+        <v>0.786218976090863</v>
+      </c>
+      <c r="K4" s="18">
+        <v>0.41128551861353002</v>
+      </c>
+      <c r="L4">
+        <v>0.63043427845966371</v>
+      </c>
+      <c r="M4" s="7">
+        <v>2.5966862137770701E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5">
+        <v>0.42848816316868665</v>
+      </c>
+      <c r="C5" s="14">
+        <v>0.33061324554751997</v>
+      </c>
+      <c r="D5">
+        <v>0.63735802226420291</v>
+      </c>
+      <c r="E5" s="15">
+        <v>0.58761063110676703</v>
+      </c>
+      <c r="F5">
+        <v>0.81423603775312137</v>
+      </c>
+      <c r="G5" s="16">
+        <v>0.876273721691745</v>
+      </c>
+      <c r="H5">
+        <v>0.99054241636648455</v>
+      </c>
+      <c r="I5" s="17">
+        <v>0.12610118972802201</v>
+      </c>
+      <c r="J5">
+        <v>0.45888690006942806</v>
+      </c>
+      <c r="K5" s="18">
+        <v>0.84451617033304205</v>
+      </c>
+      <c r="L5">
+        <v>0.27201991208227633</v>
+      </c>
+      <c r="M5" s="19">
+        <v>0.34787221257796602</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6">
+        <v>0.5397219177628636</v>
+      </c>
+      <c r="C6" s="14">
+        <v>0.41886387925431101</v>
+      </c>
+      <c r="D6">
+        <v>0.22659727426303131</v>
+      </c>
+      <c r="E6" s="15">
+        <v>0.54683519144140802</v>
+      </c>
+      <c r="F6">
+        <v>0.35326105333333335</v>
+      </c>
+      <c r="G6" s="16">
+        <v>0.60936795919082498</v>
+      </c>
+      <c r="H6">
+        <v>0.21111798635813728</v>
+      </c>
+      <c r="I6" s="17">
+        <v>0.51888455220311103</v>
+      </c>
+      <c r="J6">
+        <v>0.32106559279268015</v>
+      </c>
+      <c r="K6" s="18">
+        <v>0.92811381976317897</v>
+      </c>
+      <c r="L6">
+        <v>0.14310423164613478</v>
+      </c>
+      <c r="M6" s="19">
+        <v>0.117144834533319</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7">
+        <v>1.9945728263828013</v>
+      </c>
+      <c r="C7" s="14">
+        <v>0.73074475229926095</v>
+      </c>
+      <c r="D7">
+        <v>1.3141644952874632</v>
+      </c>
+      <c r="E7" s="15">
+        <v>0.482119508817688</v>
+      </c>
+      <c r="F7">
+        <v>0.8973491941452002</v>
+      </c>
+      <c r="G7" s="16">
+        <v>7.7299330333445299E-2</v>
+      </c>
+      <c r="H7">
+        <v>0.4916199175</v>
+      </c>
+      <c r="I7" s="17">
+        <v>0.41648763304756098</v>
+      </c>
+      <c r="J7">
+        <v>1.6020374454172757</v>
+      </c>
+      <c r="K7" s="18">
+        <v>0.92618166088133702</v>
+      </c>
+      <c r="L7">
+        <v>0.5003549260121124</v>
+      </c>
+      <c r="M7" s="7">
+        <v>1.5741522728162101E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8">
+        <v>0.66765532210763945</v>
+      </c>
+      <c r="C8" s="12">
+        <v>3.9736164584284001E-2</v>
+      </c>
+      <c r="D8">
+        <v>0.80072097966743516</v>
+      </c>
+      <c r="E8" s="9">
+        <v>2.23753114222145E-3</v>
+      </c>
+      <c r="F8">
+        <v>0.30214396953074507</v>
+      </c>
+      <c r="G8" s="10">
+        <v>2.4759724199063201E-3</v>
+      </c>
+      <c r="H8">
+        <v>2.782313449582448</v>
+      </c>
+      <c r="I8" s="17">
+        <v>0.42442038054964198</v>
+      </c>
+      <c r="J8">
+        <v>0.5935956166666666</v>
+      </c>
+      <c r="K8" s="18">
+        <v>0.57583799773840905</v>
+      </c>
+      <c r="L8">
+        <v>0.40010634388183525</v>
+      </c>
+      <c r="M8" s="7">
+        <v>1.1238296525258799E-3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>14</v>
+      </c>
+      <c r="B9">
+        <v>0.51505925890076298</v>
+      </c>
+      <c r="C9" s="14">
+        <v>0.30555896896170998</v>
+      </c>
+      <c r="D9">
+        <v>0.2965590387969203</v>
+      </c>
+      <c r="E9" s="15">
+        <v>0.220796800536256</v>
+      </c>
+      <c r="F9">
+        <v>0.85109626104804514</v>
+      </c>
+      <c r="G9" s="16">
+        <v>0.34273266373509897</v>
+      </c>
+      <c r="H9">
+        <v>0.25892374851038946</v>
+      </c>
+      <c r="I9" s="11">
+        <v>1.6849469393969401E-2</v>
+      </c>
+      <c r="J9">
+        <v>0.57355728341907597</v>
+      </c>
+      <c r="K9" s="18">
+        <v>0.80207673397527102</v>
+      </c>
+      <c r="L9">
+        <v>0.27683637751411033</v>
+      </c>
+      <c r="M9" s="19">
+        <v>8.3557084326203193E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>15</v>
+      </c>
+      <c r="B10">
+        <v>0.99071083478405697</v>
+      </c>
+      <c r="C10" s="14">
+        <v>0.40967747091093998</v>
+      </c>
+      <c r="D10">
+        <v>0.26963339746562909</v>
+      </c>
+      <c r="E10" s="9">
+        <v>4.93615335741312E-2</v>
+      </c>
+      <c r="F10">
+        <v>0.96053451505978282</v>
+      </c>
+      <c r="G10" s="16">
+        <v>7.5060611423136706E-2</v>
+      </c>
+      <c r="H10">
+        <v>0.18425456771333773</v>
+      </c>
+      <c r="I10" s="17">
+        <v>5.3349459021998002E-2</v>
+      </c>
+      <c r="J10">
+        <v>1.1729183777973196</v>
+      </c>
+      <c r="K10" s="18">
+        <v>0.83537027035042999</v>
+      </c>
+      <c r="L10">
+        <v>0.30456166505688059</v>
+      </c>
+      <c r="M10" s="7">
+        <v>2.0751052693414899E-3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>16</v>
+      </c>
+      <c r="B11">
+        <v>2.1657954209185526</v>
+      </c>
+      <c r="C11" s="14">
+        <v>0.312866167848105</v>
+      </c>
+      <c r="D11">
+        <v>0.96916677304566357</v>
+      </c>
+      <c r="E11" s="15">
+        <v>0.36919882166698498</v>
+      </c>
+      <c r="F11">
+        <v>0.23571057258955097</v>
+      </c>
+      <c r="G11" s="16">
+        <v>0.32044779172975002</v>
+      </c>
+      <c r="H11">
+        <v>0.15808487198778842</v>
+      </c>
+      <c r="I11" s="17">
+        <v>1.01926877470356</v>
+      </c>
+      <c r="J11">
+        <v>0.59558829079820264</v>
+      </c>
+      <c r="K11" s="18">
+        <v>0.41730594570108798</v>
+      </c>
+      <c r="L11">
+        <v>1.2991085393720161</v>
+      </c>
+      <c r="M11" s="19">
+        <v>0.32964773522541801</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>17</v>
+      </c>
+      <c r="B12">
+        <v>0.34789114897759943</v>
+      </c>
+      <c r="C12" s="14">
+        <v>0.673063017606508</v>
+      </c>
+      <c r="D12">
+        <v>0.64306593567178694</v>
+      </c>
+      <c r="E12" s="15">
+        <v>0.48391674975244903</v>
+      </c>
+      <c r="F12">
+        <v>0.38970517067689969</v>
+      </c>
+      <c r="G12" s="16">
+        <v>0.37967438937929698</v>
+      </c>
+      <c r="H12">
+        <v>0.18012664779265772</v>
+      </c>
+      <c r="I12" s="17">
+        <v>0.61551986182630103</v>
+      </c>
+      <c r="J12">
+        <v>0.26117035152119517</v>
+      </c>
+      <c r="K12" s="18">
+        <v>0.96518223885221099</v>
+      </c>
+      <c r="L12">
+        <v>0.24606557567042739</v>
+      </c>
+      <c r="M12" s="19">
+        <v>0.77989454444137896</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>18</v>
+      </c>
+      <c r="B13">
+        <v>0.48245556329333711</v>
+      </c>
+      <c r="C13" s="14">
+        <v>9.5712795892028399E-2</v>
+      </c>
+      <c r="D13">
+        <v>0.39365678412248828</v>
+      </c>
+      <c r="E13" s="15">
+        <v>0.44634237725270698</v>
+      </c>
+      <c r="F13">
+        <v>0.32392781216172728</v>
+      </c>
+      <c r="G13" s="16">
+        <v>0.31255665386579601</v>
+      </c>
+      <c r="H13">
+        <v>0.46696040278322037</v>
+      </c>
+      <c r="I13" s="17">
+        <v>0.98678976939878205</v>
+      </c>
+      <c r="J13">
+        <v>0.27201469396309813</v>
+      </c>
+      <c r="K13" s="18">
+        <v>0.517815470814041</v>
+      </c>
+      <c r="L13">
+        <v>0.32138354256143414</v>
+      </c>
+      <c r="M13" s="19">
+        <v>0.297478016852251</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>19</v>
+      </c>
+      <c r="B14">
+        <v>0.83836676724317216</v>
+      </c>
+      <c r="C14" s="14">
+        <v>0.174295602147962</v>
+      </c>
+      <c r="D14">
+        <v>0.82400461486764209</v>
+      </c>
+      <c r="E14" s="15">
+        <v>0.86844583111990603</v>
+      </c>
+      <c r="F14">
+        <v>0.67360449560931046</v>
+      </c>
+      <c r="G14" s="10">
+        <v>4.3268390080787603E-2</v>
+      </c>
+      <c r="H14">
+        <v>0.3378379172501691</v>
+      </c>
+      <c r="I14" s="11">
+        <v>8.3521584494051695E-3</v>
+      </c>
+      <c r="J14">
+        <v>0.36708928742273922</v>
+      </c>
+      <c r="K14" s="18">
+        <v>0.81524617305381997</v>
+      </c>
+      <c r="L14">
+        <v>0.74608708067586971</v>
+      </c>
+      <c r="M14" s="19">
+        <v>6.5292475138674894E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>20</v>
+      </c>
+      <c r="B15">
+        <v>0.40046452384198683</v>
+      </c>
+      <c r="C15" s="12">
+        <v>4.0424970068182499E-3</v>
+      </c>
+      <c r="D15">
+        <v>0.94612224295791403</v>
+      </c>
+      <c r="E15" s="15">
+        <v>5.7965913592618802E-2</v>
+      </c>
+      <c r="F15">
+        <v>0.85074359466406813</v>
+      </c>
+      <c r="G15" s="16">
+        <v>0.218104991549528</v>
+      </c>
+      <c r="H15">
+        <v>0.90546523531716228</v>
+      </c>
+      <c r="I15" s="11">
+        <v>1.17388410353965E-2</v>
+      </c>
+      <c r="J15">
+        <v>0.69744931893840034</v>
+      </c>
+      <c r="K15" s="18">
+        <v>0.21974386864794401</v>
+      </c>
+      <c r="L15">
+        <v>0.65960686937972579</v>
+      </c>
+      <c r="M15" s="19">
+        <v>0.26584607245743602</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>21</v>
+      </c>
+      <c r="B16">
+        <v>2.1737019881306301</v>
+      </c>
+      <c r="C16" s="12">
+        <v>8.8957362296602296E-3</v>
+      </c>
+      <c r="D16">
+        <v>0.67445586136967028</v>
+      </c>
+      <c r="E16" s="15">
+        <v>0.31603437363464698</v>
+      </c>
+      <c r="F16">
+        <v>0.75654832053716115</v>
+      </c>
+      <c r="G16" s="16">
+        <v>0.250267714639267</v>
+      </c>
+      <c r="H16">
+        <v>1.0283791644274656</v>
+      </c>
+      <c r="I16" s="17">
+        <v>1.01343777505961</v>
+      </c>
+      <c r="J16">
+        <v>0.54053680825347772</v>
+      </c>
+      <c r="K16" s="18">
+        <v>0.88243598341370999</v>
+      </c>
+      <c r="L16">
+        <v>3.1590337508333337</v>
+      </c>
+      <c r="M16" s="19">
+        <v>0.45617091532496501</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>7</v>
+      </c>
+      <c r="B21">
+        <f>B2-dhap4!B2</f>
+        <v>0.10381159935847911</v>
+      </c>
+      <c r="D21">
+        <f>D2-dhap4!D2</f>
+        <v>5.7348007119673333E-2</v>
+      </c>
+      <c r="F21">
+        <f>F2-dhap4!F2</f>
+        <v>3.1478895009360741E-2</v>
+      </c>
+      <c r="H21">
+        <f>H2-dhap4!H2</f>
+        <v>-3.8269226945846876E-2</v>
+      </c>
+      <c r="J21">
+        <f>J2-dhap4!J2</f>
+        <v>4.654614389168088E-3</v>
+      </c>
+      <c r="L21">
+        <f>L2-dhap4!L2</f>
+        <v>0.1689680587672977</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>8</v>
+      </c>
+      <c r="B22">
+        <f>B3-dhap4!B3</f>
+        <v>4.8217730810134196E-2</v>
+      </c>
+      <c r="D22">
+        <f>D3-dhap4!D3</f>
+        <v>0.48924611856188532</v>
+      </c>
+      <c r="F22">
+        <f>F3-dhap4!F3</f>
+        <v>-8.835392801958375E-2</v>
+      </c>
+      <c r="H22">
+        <f>H3-dhap4!H3</f>
+        <v>6.6191753168115763E-2</v>
+      </c>
+      <c r="J22">
+        <f>J3-dhap4!J3</f>
+        <v>1.0562438188892465E-3</v>
+      </c>
+      <c r="L22">
+        <f>L3-dhap4!L3</f>
+        <v>5.0361473574420001E-2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>9</v>
+      </c>
+      <c r="B23">
+        <f>B4-dhap4!B4</f>
+        <v>-0.22938688770399396</v>
+      </c>
+      <c r="D23">
+        <f>D4-dhap4!D4</f>
+        <v>0</v>
+      </c>
+      <c r="F23">
+        <f>F4-dhap4!F4</f>
+        <v>0.31246408053259511</v>
+      </c>
+      <c r="H23">
+        <f>H4-dhap4!H4</f>
+        <v>-0.15584807185965766</v>
+      </c>
+      <c r="J23">
+        <f>J4-dhap4!J4</f>
+        <v>1.6503812112054206E-2</v>
+      </c>
+      <c r="L23">
+        <f>L4-dhap4!L4</f>
+        <v>-4.7028602782133277E-2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>10</v>
+      </c>
+      <c r="B24">
+        <f>B5-dhap4!B5</f>
+        <v>-8.3539164706519897E-2</v>
+      </c>
+      <c r="D24">
+        <f>D5-dhap4!D5</f>
+        <v>-0.2665676217890941</v>
+      </c>
+      <c r="F24">
+        <f>F5-dhap4!F5</f>
+        <v>4.5058756370192299E-2</v>
+      </c>
+      <c r="H24">
+        <f>H5-dhap4!H5</f>
+        <v>0.10481469717413394</v>
+      </c>
+      <c r="J24">
+        <f>J5-dhap4!J5</f>
+        <v>-4.4400924028096089E-2</v>
+      </c>
+      <c r="L24">
+        <f>L5-dhap4!L5</f>
+        <v>4.3315889447416128E-2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>11</v>
+      </c>
+      <c r="B25">
+        <f>B6-dhap4!B6</f>
+        <v>6.5394366185710373E-2</v>
+      </c>
+      <c r="D25">
+        <f>D6-dhap4!D6</f>
+        <v>2.5198956821018775E-2</v>
+      </c>
+      <c r="F25">
+        <f>F6-dhap4!F6</f>
+        <v>0</v>
+      </c>
+      <c r="H25">
+        <f>H6-dhap4!H6</f>
+        <v>2.4358753240616399E-2</v>
+      </c>
+      <c r="J25">
+        <f>J6-dhap4!J6</f>
+        <v>8.4018782697267091E-2</v>
+      </c>
+      <c r="L25">
+        <f>L6-dhap4!L6</f>
+        <v>-2.9116794800785356E-2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>12</v>
+      </c>
+      <c r="B26">
+        <f>B7-dhap4!B7</f>
+        <v>-0.15554384596804582</v>
+      </c>
+      <c r="D26">
+        <f>D7-dhap4!D7</f>
+        <v>0.15313651058397881</v>
+      </c>
+      <c r="F26">
+        <f>F7-dhap4!F7</f>
+        <v>-0.44724623857477408</v>
+      </c>
+      <c r="H26">
+        <f>H7-dhap4!H7</f>
+        <v>0</v>
+      </c>
+      <c r="J26">
+        <f>J7-dhap4!J7</f>
+        <v>0.18065120373257737</v>
+      </c>
+      <c r="L26">
+        <f>L7-dhap4!L7</f>
+        <v>-5.931515297377965E-2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>13</v>
+      </c>
+      <c r="B27">
+        <f>B8-dhap4!B8</f>
+        <v>4.9914023054554502E-2</v>
+      </c>
+      <c r="D27">
+        <f>D8-dhap4!D8</f>
+        <v>0.11666558764381862</v>
+      </c>
+      <c r="F27">
+        <f>F8-dhap4!F8</f>
+        <v>5.4248544885031058E-3</v>
+      </c>
+      <c r="H27">
+        <f>H8-dhap4!H8</f>
+        <v>-4.5321833676129852E-2</v>
+      </c>
+      <c r="J27">
+        <f>J8-dhap4!J8</f>
+        <v>0</v>
+      </c>
+      <c r="L27">
+        <f>L8-dhap4!L8</f>
+        <v>-0.1238108281933516</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>14</v>
+      </c>
+      <c r="B28">
+        <f>B9-dhap4!B9</f>
+        <v>5.1588112041691503E-2</v>
+      </c>
+      <c r="D28">
+        <f>D9-dhap4!D9</f>
+        <v>-8.8107838662787819E-2</v>
+      </c>
+      <c r="F28">
+        <f>F9-dhap4!F9</f>
+        <v>8.1791421221698801E-2</v>
+      </c>
+      <c r="H28">
+        <f>H9-dhap4!H9</f>
+        <v>5.201268056283348E-2</v>
+      </c>
+      <c r="J28">
+        <f>J9-dhap4!J9</f>
+        <v>0.12454074149895261</v>
+      </c>
+      <c r="L28">
+        <f>L9-dhap4!L9</f>
+        <v>2.687362882630831E-2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>15</v>
+      </c>
+      <c r="B29">
+        <f>B10-dhap4!B10</f>
+        <v>8.2319513631126107E-3</v>
+      </c>
+      <c r="D29">
+        <f>D10-dhap4!D10</f>
+        <v>-3.598717269873114E-2</v>
+      </c>
+      <c r="F29">
+        <f>F10-dhap4!F10</f>
+        <v>-1.0087043926172545E-2</v>
+      </c>
+      <c r="H29">
+        <f>H10-dhap4!H10</f>
+        <v>6.0674468249886371E-3</v>
+      </c>
+      <c r="J29">
+        <f>J10-dhap4!J10</f>
+        <v>-1.276827299169403E-2</v>
+      </c>
+      <c r="L29">
+        <f>L10-dhap4!L10</f>
+        <v>3.4804761926458205E-2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>16</v>
+      </c>
+      <c r="B30">
+        <f>B11-dhap4!B11</f>
+        <v>0.36944804033610001</v>
+      </c>
+      <c r="D30">
+        <f>D11-dhap4!D11</f>
+        <v>9.3036602171663985E-2</v>
+      </c>
+      <c r="F30">
+        <f>F11-dhap4!F11</f>
+        <v>-0.15329193009537434</v>
+      </c>
+      <c r="H30">
+        <f>H11-dhap4!H11</f>
+        <v>-1.5893675590740702E-2</v>
+      </c>
+      <c r="J30">
+        <f>J11-dhap4!J11</f>
+        <v>6.1838937576249697E-2</v>
+      </c>
+      <c r="L30">
+        <f>L11-dhap4!L11</f>
+        <v>-4.8341379121121797E-2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>17</v>
+      </c>
+      <c r="B31">
+        <f>B12-dhap4!B12</f>
+        <v>3.8873618679618027E-2</v>
+      </c>
+      <c r="D31">
+        <f>D12-dhap4!D12</f>
+        <v>-5.5487577168423785E-2</v>
+      </c>
+      <c r="F31">
+        <f>F12-dhap4!F12</f>
+        <v>-7.9935791325307204E-2</v>
+      </c>
+      <c r="H31">
+        <f>H12-dhap4!H12</f>
+        <v>-1.0991428969598871E-2</v>
+      </c>
+      <c r="J31">
+        <f>J12-dhap4!J12</f>
+        <v>-5.8930181232855483E-2</v>
+      </c>
+      <c r="L31">
+        <f>L12-dhap4!L12</f>
+        <v>-2.3832793228401039E-4</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>18</v>
+      </c>
+      <c r="B32">
+        <f>B13-dhap4!B13</f>
+        <v>7.8864663152329595E-2</v>
+      </c>
+      <c r="D32">
+        <f>D13-dhap4!D13</f>
+        <v>0.167454642431523</v>
+      </c>
+      <c r="F32">
+        <f>F13-dhap4!F13</f>
+        <v>4.3713845113009075E-2</v>
+      </c>
+      <c r="H32">
+        <f>H13-dhap4!H13</f>
+        <v>2.4702914952952071E-3</v>
+      </c>
+      <c r="J32">
+        <f>J13-dhap4!J13</f>
+        <v>3.1009710709337279E-2</v>
+      </c>
+      <c r="L32">
+        <f>L13-dhap4!L13</f>
+        <v>6.9059018601917432E-3</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>19</v>
+      </c>
+      <c r="B33">
+        <f>B14-dhap4!B14</f>
+        <v>0.10431140162088881</v>
+      </c>
+      <c r="D33">
+        <f>D14-dhap4!D14</f>
+        <v>0.20026651151754349</v>
+      </c>
+      <c r="F33">
+        <f>F14-dhap4!F14</f>
+        <v>-0.36878066792108177</v>
+      </c>
+      <c r="H33">
+        <f>H14-dhap4!H14</f>
+        <v>8.4294502374637204E-2</v>
+      </c>
+      <c r="J33">
+        <f>J14-dhap4!J14</f>
+        <v>8.0289212975577229E-2</v>
+      </c>
+      <c r="L33">
+        <f>L14-dhap4!L14</f>
+        <v>0.21868434991868946</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>20</v>
+      </c>
+      <c r="B34">
+        <f>B15-dhap4!B15</f>
+        <v>-4.4391160148250508E-3</v>
+      </c>
+      <c r="D34">
+        <f>D15-dhap4!D15</f>
+        <v>0.21220824990707887</v>
+      </c>
+      <c r="F34">
+        <f>F15-dhap4!F15</f>
+        <v>-0.63817683128785763</v>
+      </c>
+      <c r="H34">
+        <f>H15-dhap4!H15</f>
+        <v>0.18160779471485577</v>
+      </c>
+      <c r="J34">
+        <f>J15-dhap4!J15</f>
+        <v>3.655726191244657E-2</v>
+      </c>
+      <c r="L34">
+        <f>L15-dhap4!L15</f>
+        <v>0.15562644337872045</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>21</v>
+      </c>
+      <c r="B35">
+        <f>B16-dhap4!B16</f>
+        <v>-0.13003769709462576</v>
+      </c>
+      <c r="D35">
+        <f>D16-dhap4!D16</f>
+        <v>9.9752662012297932E-4</v>
+      </c>
+      <c r="F35">
+        <f>F16-dhap4!F16</f>
+        <v>-0.5236715517673155</v>
+      </c>
+      <c r="H35">
+        <f>H16-dhap4!H16</f>
+        <v>-0.10039144534606836</v>
+      </c>
+      <c r="J35">
+        <f>J16-dhap4!J16</f>
+        <v>7.9679671709575184E-2</v>
+      </c>
+      <c r="L35">
+        <f>L16-dhap4!L16</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <v>1.4434426448330233</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:M38"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
       <selection activeCell="A38" sqref="A38"/>
     </sheetView>
   </sheetViews>
@@ -32026,37 +33189,37 @@
         <v>7</v>
       </c>
       <c r="B2">
-        <v>0.51820630315546445</v>
+        <v>0.46112215208604906</v>
       </c>
       <c r="C2" s="14">
         <v>0.762384490029694</v>
       </c>
       <c r="D2">
-        <v>0.15342967430076551</v>
+        <v>0.11409691296463131</v>
       </c>
       <c r="E2" s="15">
         <v>0.44624975588118598</v>
       </c>
       <c r="F2">
-        <v>1.3375201575909201</v>
+        <v>1.4547938266046232</v>
       </c>
       <c r="G2" s="16">
         <v>0.78551996118716705</v>
       </c>
       <c r="H2">
-        <v>0.10769502062634854</v>
+        <v>0.11492191751975989</v>
       </c>
       <c r="I2" s="17">
         <v>0.29160072506103601</v>
       </c>
       <c r="J2">
-        <v>0.21526229159377588</v>
+        <v>0.2035385812881898</v>
       </c>
       <c r="K2" s="18">
         <v>0.82577386681059695</v>
       </c>
       <c r="L2">
-        <v>1.0159260346188708</v>
+        <v>1.1227971509356298</v>
       </c>
       <c r="M2" s="7">
         <v>4.5710095337786E-2</v>
@@ -32067,37 +33230,37 @@
         <v>8</v>
       </c>
       <c r="B3">
-        <v>0.30180799437297201</v>
+        <v>0.48974533391701808</v>
       </c>
       <c r="C3" s="14">
         <v>8.2901279432195593E-2</v>
       </c>
       <c r="D3">
-        <v>0.78961568801773474</v>
+        <v>0.29644863888675604</v>
       </c>
       <c r="E3" s="9">
         <v>9.0782211164155292E-3</v>
       </c>
       <c r="F3">
-        <v>0.54591947676929864</v>
+        <v>0.45852618353622643</v>
       </c>
       <c r="G3" s="16">
         <v>0.52024738694317496</v>
       </c>
       <c r="H3">
-        <v>0.38238981323261939</v>
+        <v>0.67278972350758515</v>
       </c>
       <c r="I3" s="17">
         <v>7.2269282640789106E-2</v>
       </c>
       <c r="J3">
-        <v>1.1943672882960155</v>
+        <v>1.3052211266823768</v>
       </c>
       <c r="K3" s="18">
         <v>0.76388269721491497</v>
       </c>
       <c r="L3">
-        <v>1.2454099030617656</v>
+        <v>1.7147736783064085</v>
       </c>
       <c r="M3" s="19">
         <v>0.45347930983877699</v>
@@ -32108,7 +33271,7 @@
         <v>9</v>
       </c>
       <c r="B4">
-        <v>0.60003795339805421</v>
+        <v>0.82136656767930671</v>
       </c>
       <c r="C4" s="14">
         <v>6.6225124959576706E-2</v>
@@ -32120,25 +33283,25 @@
         <v>0.61881514010194805</v>
       </c>
       <c r="F4">
-        <v>1.1803841392068706</v>
+        <v>0.87911802750831702</v>
       </c>
       <c r="G4" s="10">
         <v>1.6347989883004101E-2</v>
       </c>
       <c r="H4">
-        <v>0.93850425171750873</v>
+        <v>1.2424380752332995</v>
       </c>
       <c r="I4" s="11">
         <v>1.1178235493982801E-2</v>
       </c>
       <c r="J4">
-        <v>0.786218976090863</v>
+        <v>0.76544302081760351</v>
       </c>
       <c r="K4" s="18">
         <v>0.41128551861353002</v>
       </c>
       <c r="L4">
-        <v>0.63043427845966371</v>
+        <v>0.57120805224265481</v>
       </c>
       <c r="M4" s="7">
         <v>2.5966862137770701E-2</v>
@@ -32149,37 +33312,37 @@
         <v>10</v>
       </c>
       <c r="B5">
-        <v>0.42848816316868665</v>
+        <v>0.52688788457775138</v>
       </c>
       <c r="C5" s="14">
         <v>0.33061324554751997</v>
       </c>
       <c r="D5">
-        <v>0.63735802226420291</v>
+        <v>0.64669699544140891</v>
       </c>
       <c r="E5" s="15">
         <v>0.58761063110676703</v>
       </c>
       <c r="F5">
-        <v>0.81423603775312137</v>
+        <v>0.7924598779437847</v>
       </c>
       <c r="G5" s="16">
         <v>0.876273721691745</v>
       </c>
       <c r="H5">
-        <v>0.99054241636648455</v>
+        <v>0.96389246062592626</v>
       </c>
       <c r="I5" s="17">
         <v>0.12610118972802201</v>
       </c>
       <c r="J5">
-        <v>0.45888690006942806</v>
+        <v>0.45662803886995179</v>
       </c>
       <c r="K5" s="18">
         <v>0.84451617033304205</v>
       </c>
       <c r="L5">
-        <v>0.27201991208227633</v>
+        <v>0.24064452764194477</v>
       </c>
       <c r="M5" s="19">
         <v>0.34787221257796602</v>
@@ -32190,13 +33353,13 @@
         <v>11</v>
       </c>
       <c r="B6">
-        <v>0.5397219177628636</v>
+        <v>0.53963272401171725</v>
       </c>
       <c r="C6" s="14">
         <v>0.41886387925431101</v>
       </c>
       <c r="D6">
-        <v>0.22659727426303131</v>
+        <v>0.22687610353691937</v>
       </c>
       <c r="E6" s="15">
         <v>0.54683519144140802</v>
@@ -32208,19 +33371,19 @@
         <v>0.60936795919082498</v>
       </c>
       <c r="H6">
-        <v>0.21111798635813728</v>
+        <v>0.21108892083843003</v>
       </c>
       <c r="I6" s="17">
         <v>0.51888455220311103</v>
       </c>
       <c r="J6">
-        <v>0.32106559279268015</v>
+        <v>0.32055488791186487</v>
       </c>
       <c r="K6" s="18">
         <v>0.92811381976317897</v>
       </c>
       <c r="L6">
-        <v>0.14310423164613478</v>
+        <v>0.14344976181795074</v>
       </c>
       <c r="M6" s="19">
         <v>0.117144834533319</v>
@@ -32231,19 +33394,19 @@
         <v>12</v>
       </c>
       <c r="B7">
-        <v>1.9945728263828013</v>
+        <v>1.8577549561755891</v>
       </c>
       <c r="C7" s="14">
         <v>0.73074475229926095</v>
       </c>
       <c r="D7">
-        <v>1.3141644952874632</v>
+        <v>1.2085765355786768</v>
       </c>
       <c r="E7" s="15">
         <v>0.482119508817688</v>
       </c>
       <c r="F7">
-        <v>0.8973491941452002</v>
+        <v>0.76855165632996802</v>
       </c>
       <c r="G7" s="16">
         <v>7.7299330333445299E-2</v>
@@ -32255,13 +33418,13 @@
         <v>0.41648763304756098</v>
       </c>
       <c r="J7">
-        <v>1.6020374454172757</v>
+        <v>1.3783372471540114</v>
       </c>
       <c r="K7" s="18">
         <v>0.92618166088133702</v>
       </c>
       <c r="L7">
-        <v>0.5003549260121124</v>
+        <v>0.6610084249152951</v>
       </c>
       <c r="M7" s="7">
         <v>1.5741522728162101E-2</v>
@@ -32272,25 +33435,25 @@
         <v>13</v>
       </c>
       <c r="B8">
-        <v>0.66765532210763945</v>
+        <v>0.65821465139042301</v>
       </c>
       <c r="C8" s="12">
         <v>3.9736164584284001E-2</v>
       </c>
       <c r="D8">
-        <v>0.80072097966743516</v>
+        <v>0.71702453227371521</v>
       </c>
       <c r="E8" s="9">
         <v>2.23753114222145E-3</v>
       </c>
       <c r="F8">
-        <v>0.30214396953074507</v>
+        <v>0.3087062566091146</v>
       </c>
       <c r="G8" s="10">
         <v>2.4759724199063201E-3</v>
       </c>
       <c r="H8">
-        <v>2.782313449582448</v>
+        <v>2.7472229191422368</v>
       </c>
       <c r="I8" s="17">
         <v>0.42442038054964198</v>
@@ -32302,7 +33465,7 @@
         <v>0.57583799773840905</v>
       </c>
       <c r="L8">
-        <v>0.40010634388183525</v>
+        <v>0.39758210802947591</v>
       </c>
       <c r="M8" s="7">
         <v>1.1238296525258799E-3</v>
@@ -32313,37 +33476,37 @@
         <v>14</v>
       </c>
       <c r="B9">
-        <v>0.51505925890076298</v>
+        <v>0.4839265757631081</v>
       </c>
       <c r="C9" s="14">
         <v>0.30555896896170998</v>
       </c>
       <c r="D9">
-        <v>0.2965590387969203</v>
+        <v>0.24300740668104748</v>
       </c>
       <c r="E9" s="15">
         <v>0.220796800536256</v>
       </c>
       <c r="F9">
-        <v>0.85109626104804514</v>
+        <v>0.76385348049111823</v>
       </c>
       <c r="G9" s="16">
         <v>0.34273266373509897</v>
       </c>
       <c r="H9">
-        <v>0.25892374851038946</v>
+        <v>0.19594449143337758</v>
       </c>
       <c r="I9" s="11">
         <v>1.6849469393969401E-2</v>
       </c>
       <c r="J9">
-        <v>0.57355728341907597</v>
+        <v>0.38521858272591453</v>
       </c>
       <c r="K9" s="18">
         <v>0.80207673397527102</v>
       </c>
       <c r="L9">
-        <v>0.27683637751411033</v>
+        <v>0.278061831236255</v>
       </c>
       <c r="M9" s="19">
         <v>8.3557084326203193E-2</v>
@@ -32354,37 +33517,37 @@
         <v>15</v>
       </c>
       <c r="B10">
-        <v>0.99071083478405697</v>
+        <v>0.99028608491458492</v>
       </c>
       <c r="C10" s="14">
         <v>0.40967747091093998</v>
       </c>
       <c r="D10">
-        <v>0.26963339746562909</v>
+        <v>0.27225886781414432</v>
       </c>
       <c r="E10" s="9">
         <v>4.93615335741312E-2</v>
       </c>
       <c r="F10">
-        <v>0.96053451505978282</v>
+        <v>0.96456717952740434</v>
       </c>
       <c r="G10" s="16">
         <v>7.5060611423136706E-2</v>
       </c>
       <c r="H10">
-        <v>0.18425456771333773</v>
+        <v>0.18153217623684234</v>
       </c>
       <c r="I10" s="17">
         <v>5.3349459021998002E-2</v>
       </c>
       <c r="J10">
-        <v>1.1729183777973196</v>
+        <v>1.1806343885973651</v>
       </c>
       <c r="K10" s="18">
         <v>0.83537027035042999</v>
       </c>
       <c r="L10">
-        <v>0.30456166505688059</v>
+        <v>0.3024961994296394</v>
       </c>
       <c r="M10" s="7">
         <v>2.0751052693414899E-3</v>
@@ -32395,37 +33558,37 @@
         <v>16</v>
       </c>
       <c r="B11">
-        <v>2.1657954209185526</v>
+        <v>1.7113981939566447</v>
       </c>
       <c r="C11" s="14">
         <v>0.312866167848105</v>
       </c>
       <c r="D11">
-        <v>0.96916677304566357</v>
+        <v>0.89104278322303887</v>
       </c>
       <c r="E11" s="15">
         <v>0.36919882166698498</v>
       </c>
       <c r="F11">
-        <v>0.23571057258955097</v>
+        <v>0.44385243511702721</v>
       </c>
       <c r="G11" s="16">
         <v>0.32044779172975002</v>
       </c>
       <c r="H11">
-        <v>0.15808487198778842</v>
+        <v>0.14343727145828514</v>
       </c>
       <c r="I11" s="17">
         <v>1.01926877470356</v>
       </c>
       <c r="J11">
-        <v>0.59558829079820264</v>
+        <v>0.47454350082757868</v>
       </c>
       <c r="K11" s="18">
         <v>0.41730594570108798</v>
       </c>
       <c r="L11">
-        <v>1.2991085393720161</v>
+        <v>1.297413474292761</v>
       </c>
       <c r="M11" s="19">
         <v>0.32964773522541801</v>
@@ -32436,37 +33599,37 @@
         <v>17</v>
       </c>
       <c r="B12">
-        <v>0.34789114897759943</v>
+        <v>0.29688838031233133</v>
       </c>
       <c r="C12" s="14">
         <v>0.673063017606508</v>
       </c>
       <c r="D12">
-        <v>0.64306593567178694</v>
+        <v>0.73874052389088429</v>
       </c>
       <c r="E12" s="15">
         <v>0.48391674975244903</v>
       </c>
       <c r="F12">
-        <v>0.38970517067689969</v>
+        <v>0.46209498663920695</v>
       </c>
       <c r="G12" s="16">
         <v>0.37967438937929698</v>
       </c>
       <c r="H12">
-        <v>0.18012664779265772</v>
+        <v>0.27735704068119521</v>
       </c>
       <c r="I12" s="17">
         <v>0.61551986182630103</v>
       </c>
       <c r="J12">
-        <v>0.26117035152119517</v>
+        <v>0.23854582656251241</v>
       </c>
       <c r="K12" s="18">
         <v>0.96518223885221099</v>
       </c>
       <c r="L12">
-        <v>0.24606557567042739</v>
+        <v>0.30686641808190623</v>
       </c>
       <c r="M12" s="19">
         <v>0.77989454444137896</v>
@@ -32477,37 +33640,37 @@
         <v>18</v>
       </c>
       <c r="B13">
-        <v>0.48245556329333711</v>
+        <v>0.42738449183520977</v>
       </c>
       <c r="C13" s="14">
         <v>9.5712795892028399E-2</v>
       </c>
       <c r="D13">
-        <v>0.39365678412248828</v>
+        <v>0.21362780326051678</v>
       </c>
       <c r="E13" s="15">
         <v>0.44634237725270698</v>
       </c>
       <c r="F13">
-        <v>0.32392781216172728</v>
+        <v>0.26820748544976547</v>
       </c>
       <c r="G13" s="16">
         <v>0.31255665386579601</v>
       </c>
       <c r="H13">
-        <v>0.46696040278322037</v>
+        <v>0.49638463267009647</v>
       </c>
       <c r="I13" s="17">
         <v>0.98678976939878205</v>
       </c>
       <c r="J13">
-        <v>0.27201469396309813</v>
+        <v>0.26816112269166736</v>
       </c>
       <c r="K13" s="18">
         <v>0.517815470814041</v>
       </c>
       <c r="L13">
-        <v>0.32138354256143414</v>
+        <v>0.26500577435882161</v>
       </c>
       <c r="M13" s="19">
         <v>0.297478016852251</v>
@@ -32518,37 +33681,37 @@
         <v>19</v>
       </c>
       <c r="B14">
-        <v>0.83836676724317216</v>
+        <v>0.90774300734455626</v>
       </c>
       <c r="C14" s="14">
         <v>0.174295602147962</v>
       </c>
       <c r="D14">
-        <v>0.82400461486764209</v>
+        <v>0.66641262877798357</v>
       </c>
       <c r="E14" s="15">
         <v>0.86844583111990603</v>
       </c>
       <c r="F14">
-        <v>0.67360449560931046</v>
+        <v>1.1724805056106791</v>
       </c>
       <c r="G14" s="10">
         <v>4.3268390080787603E-2</v>
       </c>
       <c r="H14">
-        <v>0.3378379172501691</v>
+        <v>0.75208338269645891</v>
       </c>
       <c r="I14" s="11">
         <v>8.3521584494051695E-3</v>
       </c>
       <c r="J14">
-        <v>0.36708928742273922</v>
+        <v>0.43925242938827952</v>
       </c>
       <c r="K14" s="18">
         <v>0.81524617305381997</v>
       </c>
       <c r="L14">
-        <v>0.74608708067586971</v>
+        <v>0.91687737258891866</v>
       </c>
       <c r="M14" s="19">
         <v>6.5292475138674894E-2</v>
@@ -32559,37 +33722,37 @@
         <v>20</v>
       </c>
       <c r="B15">
-        <v>0.40046452384198683</v>
+        <v>0.44478698122309529</v>
       </c>
       <c r="C15" s="12">
         <v>4.0424970068182499E-3</v>
       </c>
       <c r="D15">
-        <v>0.94612224295791403</v>
+        <v>0.93149676145323135</v>
       </c>
       <c r="E15" s="15">
         <v>5.7965913592618802E-2</v>
       </c>
       <c r="F15">
-        <v>0.85074359466406813</v>
+        <v>1.426580488634615</v>
       </c>
       <c r="G15" s="16">
         <v>0.218104991549528</v>
       </c>
       <c r="H15">
-        <v>0.90546523531716228</v>
+        <v>0.88069436055912442</v>
       </c>
       <c r="I15" s="11">
         <v>1.17388410353965E-2</v>
       </c>
       <c r="J15">
-        <v>0.69744931893840034</v>
+        <v>0.73363145607850022</v>
       </c>
       <c r="K15" s="18">
         <v>0.21974386864794401</v>
       </c>
       <c r="L15">
-        <v>0.65960686937972579</v>
+        <v>0.64989997196925531</v>
       </c>
       <c r="M15" s="19">
         <v>0.26584607245743602</v>
@@ -32600,31 +33763,31 @@
         <v>21</v>
       </c>
       <c r="B16">
-        <v>2.1737019881306301</v>
+        <v>2.1646445435857284</v>
       </c>
       <c r="C16" s="12">
         <v>8.8957362296602296E-3</v>
       </c>
       <c r="D16">
-        <v>0.67445586136967028</v>
+        <v>0.64806122058364135</v>
       </c>
       <c r="E16" s="15">
         <v>0.31603437363464698</v>
       </c>
       <c r="F16">
-        <v>0.75654832053716115</v>
+        <v>1.3733968034493114</v>
       </c>
       <c r="G16" s="16">
         <v>0.250267714639267</v>
       </c>
       <c r="H16">
-        <v>1.0283791644274656</v>
+        <v>1.165314911580607</v>
       </c>
       <c r="I16" s="17">
         <v>1.01343777505961</v>
       </c>
       <c r="J16">
-        <v>0.54053680825347772</v>
+        <v>0.33866935597811709</v>
       </c>
       <c r="K16" s="18">
         <v>0.88243598341370999</v>
@@ -32636,442 +33799,442 @@
         <v>0.45617091532496501</v>
       </c>
     </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>174</v>
+      </c>
+    </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>171</v>
+        <v>7</v>
+      </c>
+      <c r="B20">
+        <f>B2-dhap4!B2</f>
+        <v>4.6727448289063722E-2</v>
+      </c>
+      <c r="D20">
+        <f>D2-dhap4!D2</f>
+        <v>1.8015245783539136E-2</v>
+      </c>
+      <c r="F20">
+        <f>F2-dhap4!F2</f>
+        <v>0.1487525640230638</v>
+      </c>
+      <c r="H20">
+        <f>H2-dhap4!H2</f>
+        <v>-3.1042330052435535E-2</v>
+      </c>
+      <c r="J20">
+        <f>J2-dhap4!J2</f>
+        <v>-7.0690959164179945E-3</v>
+      </c>
+      <c r="L20">
+        <f>L2-dhap4!L2</f>
+        <v>0.27583917508405675</v>
       </c>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B21">
-        <f>B2-dhap4!B2</f>
-        <v>0.10381159935847911</v>
+        <f>B3-dhap4!B3</f>
+        <v>0.23615507035418026</v>
       </c>
       <c r="D21">
-        <f>D2-dhap4!D2</f>
-        <v>5.7348007119673333E-2</v>
+        <f>D3-dhap4!D3</f>
+        <v>-3.9209305690933727E-3</v>
       </c>
       <c r="F21">
-        <f>F2-dhap4!F2</f>
-        <v>3.1478895009360741E-2</v>
+        <f>F3-dhap4!F3</f>
+        <v>-0.17574722125265596</v>
       </c>
       <c r="H21">
-        <f>H2-dhap4!H2</f>
-        <v>-3.8269226945846876E-2</v>
+        <f>H3-dhap4!H3</f>
+        <v>0.35659166344308152</v>
       </c>
       <c r="J21">
-        <f>J2-dhap4!J2</f>
-        <v>4.654614389168088E-3</v>
+        <f>J3-dhap4!J3</f>
+        <v>0.11191008220525056</v>
       </c>
       <c r="L21">
-        <f>L2-dhap4!L2</f>
-        <v>0.1689680587672977</v>
+        <f>L3-dhap4!L3</f>
+        <v>0.5197252488190629</v>
       </c>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B22">
-        <f>B3-dhap4!B3</f>
-        <v>4.8217730810134196E-2</v>
+        <f>B4-dhap4!B4</f>
+        <v>-8.0582734227414576E-3</v>
       </c>
       <c r="D22">
-        <f>D3-dhap4!D3</f>
-        <v>0.48924611856188532</v>
+        <f>D4-dhap4!D4</f>
+        <v>0</v>
       </c>
       <c r="F22">
-        <f>F3-dhap4!F3</f>
-        <v>-8.835392801958375E-2</v>
+        <f>F4-dhap4!F4</f>
+        <v>1.1197968834041561E-2</v>
       </c>
       <c r="H22">
-        <f>H3-dhap4!H3</f>
-        <v>6.6191753168115763E-2</v>
+        <f>H4-dhap4!H4</f>
+        <v>0.14808575165613314</v>
       </c>
       <c r="J22">
-        <f>J3-dhap4!J3</f>
-        <v>1.0562438188892465E-3</v>
+        <f>J4-dhap4!J4</f>
+        <v>-4.2721431612052774E-3</v>
       </c>
       <c r="L22">
-        <f>L3-dhap4!L3</f>
-        <v>5.0361473574420001E-2</v>
+        <f>L4-dhap4!L4</f>
+        <v>-0.10625482899914218</v>
       </c>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B23">
-        <f>B4-dhap4!B4</f>
-        <v>-0.22938688770399396</v>
+        <f>B5-dhap4!B5</f>
+        <v>1.4860556702544825E-2</v>
       </c>
       <c r="D23">
-        <f>D4-dhap4!D4</f>
-        <v>0</v>
+        <f>D5-dhap4!D5</f>
+        <v>-0.2572286486118881</v>
       </c>
       <c r="F23">
-        <f>F4-dhap4!F4</f>
-        <v>0.31246408053259511</v>
+        <f>F5-dhap4!F5</f>
+        <v>2.3282596560855628E-2</v>
       </c>
       <c r="H23">
-        <f>H4-dhap4!H4</f>
-        <v>-0.15584807185965766</v>
+        <f>H5-dhap4!H5</f>
+        <v>7.8164741433575657E-2</v>
       </c>
       <c r="J23">
-        <f>J4-dhap4!J4</f>
-        <v>1.6503812112054206E-2</v>
+        <f>J5-dhap4!J5</f>
+        <v>-4.6659785227572359E-2</v>
       </c>
       <c r="L23">
-        <f>L4-dhap4!L4</f>
-        <v>-4.7028602782133277E-2</v>
+        <f>L5-dhap4!L5</f>
+        <v>1.1940505007084573E-2</v>
       </c>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B24">
-        <f>B5-dhap4!B5</f>
-        <v>-8.3539164706519897E-2</v>
+        <f>B6-dhap4!B6</f>
+        <v>6.5305172434564018E-2</v>
       </c>
       <c r="D24">
-        <f>D5-dhap4!D5</f>
-        <v>-0.2665676217890941</v>
+        <f>D6-dhap4!D6</f>
+        <v>2.5477786094906835E-2</v>
       </c>
       <c r="F24">
-        <f>F5-dhap4!F5</f>
-        <v>4.5058756370192299E-2</v>
+        <f>F6-dhap4!F6</f>
+        <v>0</v>
       </c>
       <c r="H24">
-        <f>H5-dhap4!H5</f>
-        <v>0.10481469717413394</v>
+        <f>H6-dhap4!H6</f>
+        <v>2.4329687720909154E-2</v>
       </c>
       <c r="J24">
-        <f>J5-dhap4!J5</f>
-        <v>-4.4400924028096089E-2</v>
+        <f>J6-dhap4!J6</f>
+        <v>8.3508077816451809E-2</v>
       </c>
       <c r="L24">
-        <f>L5-dhap4!L5</f>
-        <v>4.3315889447416128E-2</v>
+        <f>L6-dhap4!L6</f>
+        <v>-2.8771264628969395E-2</v>
       </c>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B25">
-        <f>B6-dhap4!B6</f>
-        <v>6.5394366185710373E-2</v>
+        <f>B7-dhap4!B7</f>
+        <v>-0.29236171617525808</v>
       </c>
       <c r="D25">
-        <f>D6-dhap4!D6</f>
-        <v>2.5198956821018775E-2</v>
+        <f>D7-dhap4!D7</f>
+        <v>4.7548550875192497E-2</v>
       </c>
       <c r="F25">
-        <f>F6-dhap4!F6</f>
+        <f>F7-dhap4!F7</f>
+        <v>-0.57604377639000626</v>
+      </c>
+      <c r="H25">
+        <f>H7-dhap4!H7</f>
         <v>0</v>
       </c>
-      <c r="H25">
-        <f>H6-dhap4!H6</f>
-        <v>2.4358753240616399E-2</v>
-      </c>
       <c r="J25">
-        <f>J6-dhap4!J6</f>
-        <v>8.4018782697267091E-2</v>
+        <f>J7-dhap4!J7</f>
+        <v>-4.304899453068689E-2</v>
       </c>
       <c r="L25">
-        <f>L6-dhap4!L6</f>
-        <v>-2.9116794800785356E-2</v>
+        <f>L7-dhap4!L7</f>
+        <v>0.10133834592940305</v>
       </c>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B26">
-        <f>B7-dhap4!B7</f>
-        <v>-0.15554384596804582</v>
+        <f>B8-dhap4!B8</f>
+        <v>4.0473352337338064E-2</v>
       </c>
       <c r="D26">
-        <f>D7-dhap4!D7</f>
-        <v>0.15313651058397881</v>
+        <f>D8-dhap4!D8</f>
+        <v>3.2969140250098672E-2</v>
       </c>
       <c r="F26">
-        <f>F7-dhap4!F7</f>
-        <v>-0.44724623857477408</v>
+        <f>F8-dhap4!F8</f>
+        <v>1.1987141566872639E-2</v>
       </c>
       <c r="H26">
-        <f>H7-dhap4!H7</f>
+        <f>H8-dhap4!H8</f>
+        <v>-8.0412364116341006E-2</v>
+      </c>
+      <c r="J26">
+        <f>J8-dhap4!J8</f>
         <v>0</v>
       </c>
-      <c r="J26">
-        <f>J7-dhap4!J7</f>
-        <v>0.18065120373257737</v>
-      </c>
       <c r="L26">
-        <f>L7-dhap4!L7</f>
-        <v>-5.931515297377965E-2</v>
+        <f>L8-dhap4!L8</f>
+        <v>-0.12633506404571093</v>
       </c>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B27">
-        <f>B8-dhap4!B8</f>
-        <v>4.9914023054554502E-2</v>
+        <f>B9-dhap4!B9</f>
+        <v>2.0455428904036621E-2</v>
       </c>
       <c r="D27">
-        <f>D8-dhap4!D8</f>
-        <v>0.11666558764381862</v>
+        <f>D9-dhap4!D9</f>
+        <v>-0.14165947077866065</v>
       </c>
       <c r="F27">
-        <f>F8-dhap4!F8</f>
-        <v>5.4248544885031058E-3</v>
+        <f>F9-dhap4!F9</f>
+        <v>-5.451359335228112E-3</v>
       </c>
       <c r="H27">
-        <f>H8-dhap4!H8</f>
-        <v>-4.5321833676129852E-2</v>
+        <f>H9-dhap4!H9</f>
+        <v>-1.09665765141784E-2</v>
       </c>
       <c r="J27">
-        <f>J8-dhap4!J8</f>
-        <v>0</v>
+        <f>J9-dhap4!J9</f>
+        <v>-6.3797959194208831E-2</v>
       </c>
       <c r="L27">
-        <f>L8-dhap4!L8</f>
-        <v>-0.1238108281933516</v>
+        <f>L9-dhap4!L9</f>
+        <v>2.8099082548452975E-2</v>
       </c>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B28">
-        <f>B9-dhap4!B9</f>
-        <v>5.1588112041691503E-2</v>
+        <f>B10-dhap4!B10</f>
+        <v>7.8072014936405587E-3</v>
       </c>
       <c r="D28">
-        <f>D9-dhap4!D9</f>
-        <v>-8.8107838662787819E-2</v>
+        <f>D10-dhap4!D10</f>
+        <v>-3.3361702350215905E-2</v>
       </c>
       <c r="F28">
-        <f>F9-dhap4!F9</f>
-        <v>8.1791421221698801E-2</v>
+        <f>F10-dhap4!F10</f>
+        <v>-6.0543794585510291E-3</v>
       </c>
       <c r="H28">
-        <f>H9-dhap4!H9</f>
-        <v>5.201268056283348E-2</v>
+        <f>H10-dhap4!H10</f>
+        <v>3.3450553484932477E-3</v>
       </c>
       <c r="J28">
-        <f>J9-dhap4!J9</f>
-        <v>0.12454074149895261</v>
+        <f>J10-dhap4!J10</f>
+        <v>-5.0522621916484489E-3</v>
       </c>
       <c r="L28">
-        <f>L9-dhap4!L9</f>
-        <v>2.687362882630831E-2</v>
+        <f>L10-dhap4!L10</f>
+        <v>3.2739296299217013E-2</v>
       </c>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B29">
-        <f>B10-dhap4!B10</f>
-        <v>8.2319513631126107E-3</v>
+        <f>B11-dhap4!B11</f>
+        <v>-8.494918662580786E-2</v>
       </c>
       <c r="D29">
-        <f>D10-dhap4!D10</f>
-        <v>-3.598717269873114E-2</v>
+        <f>D11-dhap4!D11</f>
+        <v>1.4912612349039289E-2</v>
       </c>
       <c r="F29">
-        <f>F10-dhap4!F10</f>
-        <v>-1.0087043926172545E-2</v>
+        <f>F11-dhap4!F11</f>
+        <v>5.48499324321019E-2</v>
       </c>
       <c r="H29">
-        <f>H10-dhap4!H10</f>
-        <v>6.0674468249886371E-3</v>
+        <f>H11-dhap4!H11</f>
+        <v>-3.0541276120243988E-2</v>
       </c>
       <c r="J29">
-        <f>J10-dhap4!J10</f>
-        <v>-1.276827299169403E-2</v>
+        <f>J11-dhap4!J11</f>
+        <v>-5.9205852394374259E-2</v>
       </c>
       <c r="L29">
-        <f>L10-dhap4!L10</f>
-        <v>3.4804761926458205E-2</v>
+        <f>L11-dhap4!L11</f>
+        <v>-5.0036444200376895E-2</v>
       </c>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B30">
-        <f>B11-dhap4!B11</f>
-        <v>0.36944804033610001</v>
+        <f>B12-dhap4!B12</f>
+        <v>-1.2129149985650067E-2</v>
       </c>
       <c r="D30">
-        <f>D11-dhap4!D11</f>
-        <v>9.3036602171663985E-2</v>
+        <f>D12-dhap4!D12</f>
+        <v>4.0187011050673571E-2</v>
       </c>
       <c r="F30">
-        <f>F11-dhap4!F11</f>
-        <v>-0.15329193009537434</v>
+        <f>F12-dhap4!F12</f>
+        <v>-7.545975362999946E-3</v>
       </c>
       <c r="H30">
-        <f>H11-dhap4!H11</f>
-        <v>-1.5893675590740702E-2</v>
+        <f>H12-dhap4!H12</f>
+        <v>8.6238963918938621E-2</v>
       </c>
       <c r="J30">
-        <f>J11-dhap4!J11</f>
-        <v>6.1838937576249697E-2</v>
+        <f>J12-dhap4!J12</f>
+        <v>-8.1554706191538234E-2</v>
       </c>
       <c r="L30">
-        <f>L11-dhap4!L11</f>
-        <v>-4.8341379121121797E-2</v>
+        <f>L12-dhap4!L12</f>
+        <v>6.0562514479194834E-2</v>
       </c>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B31">
-        <f>B12-dhap4!B12</f>
-        <v>3.8873618679618027E-2</v>
+        <f>B13-dhap4!B13</f>
+        <v>2.3793591694202254E-2</v>
       </c>
       <c r="D31">
-        <f>D12-dhap4!D12</f>
-        <v>-5.5487577168423785E-2</v>
+        <f>D13-dhap4!D13</f>
+        <v>-1.2574338430448501E-2</v>
       </c>
       <c r="F31">
-        <f>F12-dhap4!F12</f>
-        <v>-7.9935791325307204E-2</v>
+        <f>F13-dhap4!F13</f>
+        <v>-1.2006481598952734E-2</v>
       </c>
       <c r="H31">
-        <f>H12-dhap4!H12</f>
-        <v>-1.0991428969598871E-2</v>
+        <f>H13-dhap4!H13</f>
+        <v>3.1894521382171304E-2</v>
       </c>
       <c r="J31">
-        <f>J12-dhap4!J12</f>
-        <v>-5.8930181232855483E-2</v>
+        <f>J13-dhap4!J13</f>
+        <v>2.7156139437906512E-2</v>
       </c>
       <c r="L31">
-        <f>L12-dhap4!L12</f>
-        <v>-2.3832793228401039E-4</v>
+        <f>L13-dhap4!L13</f>
+        <v>-4.9471866342420789E-2</v>
       </c>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B32">
-        <f>B13-dhap4!B13</f>
-        <v>7.8864663152329595E-2</v>
+        <f>B14-dhap4!B14</f>
+        <v>0.17368764172227291</v>
       </c>
       <c r="D32">
-        <f>D13-dhap4!D13</f>
-        <v>0.167454642431523</v>
+        <f>D14-dhap4!D14</f>
+        <v>4.2674525427884968E-2</v>
       </c>
       <c r="F32">
-        <f>F13-dhap4!F13</f>
-        <v>4.3713845113009075E-2</v>
+        <f>F14-dhap4!F14</f>
+        <v>0.13009534208028684</v>
       </c>
       <c r="H32">
-        <f>H13-dhap4!H13</f>
-        <v>2.4702914952952071E-3</v>
+        <f>H14-dhap4!H14</f>
+        <v>0.49853996782092702</v>
       </c>
       <c r="J32">
-        <f>J13-dhap4!J13</f>
-        <v>3.1009710709337279E-2</v>
+        <f>J14-dhap4!J14</f>
+        <v>0.15245235494111753</v>
       </c>
       <c r="L32">
-        <f>L13-dhap4!L13</f>
-        <v>6.9059018601917432E-3</v>
+        <f>L14-dhap4!L14</f>
+        <v>0.38947464183173841</v>
       </c>
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B33">
-        <f>B14-dhap4!B14</f>
-        <v>0.10431140162088881</v>
+        <f>B15-dhap4!B15</f>
+        <v>3.9883341366283409E-2</v>
       </c>
       <c r="D33">
-        <f>D14-dhap4!D14</f>
-        <v>0.20026651151754349</v>
+        <f>D15-dhap4!D15</f>
+        <v>0.19758276840239619</v>
       </c>
       <c r="F33">
-        <f>F14-dhap4!F14</f>
-        <v>-0.36878066792108177</v>
+        <f>F15-dhap4!F15</f>
+        <v>-6.2339937317310801E-2</v>
       </c>
       <c r="H33">
-        <f>H14-dhap4!H14</f>
-        <v>8.4294502374637204E-2</v>
+        <f>H15-dhap4!H15</f>
+        <v>0.15683691995681792</v>
       </c>
       <c r="J33">
-        <f>J14-dhap4!J14</f>
-        <v>8.0289212975577229E-2</v>
+        <f>J15-dhap4!J15</f>
+        <v>7.273939905254645E-2</v>
       </c>
       <c r="L33">
-        <f>L14-dhap4!L14</f>
-        <v>0.21868434991868946</v>
+        <f>L15-dhap4!L15</f>
+        <v>0.14591954596824996</v>
       </c>
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B34">
-        <f>B15-dhap4!B15</f>
-        <v>-4.4391160148250508E-3</v>
+        <f>B16-dhap4!B16</f>
+        <v>-0.13909514163952741</v>
       </c>
       <c r="D34">
-        <f>D15-dhap4!D15</f>
-        <v>0.21220824990707887</v>
+        <f>D16-dhap4!D16</f>
+        <v>-2.5397114165905954E-2</v>
       </c>
       <c r="F34">
-        <f>F15-dhap4!F15</f>
-        <v>-0.63817683128785763</v>
+        <f>F16-dhap4!F16</f>
+        <v>9.3176931144834718E-2</v>
       </c>
       <c r="H34">
-        <f>H15-dhap4!H15</f>
-        <v>0.18160779471485577</v>
+        <f>H16-dhap4!H16</f>
+        <v>3.6544301807073021E-2</v>
       </c>
       <c r="J34">
-        <f>J15-dhap4!J15</f>
-        <v>3.655726191244657E-2</v>
+        <f>J16-dhap4!J16</f>
+        <v>-0.12218778056578544</v>
       </c>
       <c r="L34">
-        <f>L15-dhap4!L15</f>
-        <v>0.15562644337872045</v>
-      </c>
-    </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
-        <v>21</v>
-      </c>
-      <c r="B35">
-        <f>B16-dhap4!B16</f>
-        <v>-0.13003769709462576</v>
-      </c>
-      <c r="D35">
-        <f>D16-dhap4!D16</f>
-        <v>9.9752662012297932E-4</v>
-      </c>
-      <c r="F35">
-        <f>F16-dhap4!F16</f>
-        <v>-0.5236715517673155</v>
-      </c>
-      <c r="H35">
-        <f>H16-dhap4!H16</f>
-        <v>-0.10039144534606836</v>
-      </c>
-      <c r="J35">
-        <f>J16-dhap4!J16</f>
-        <v>7.9679671709575184E-2</v>
-      </c>
-      <c r="L35">
         <f>L16-dhap4!L16</f>
         <v>0</v>
       </c>
@@ -33083,342 +34246,7 @@
     </row>
     <row r="38" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A38">
-        <v>1.4434426448330233</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="N1:S16"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="N1" sqref="N1:S16"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="14:19" x14ac:dyDescent="0.25">
-      <c r="N1" s="14" t="s">
-        <v>22</v>
-      </c>
-      <c r="O1" s="15" t="s">
-        <v>23</v>
-      </c>
-      <c r="P1" s="16" t="s">
-        <v>24</v>
-      </c>
-      <c r="Q1" s="17" t="s">
-        <v>25</v>
-      </c>
-      <c r="R1" s="18" t="s">
-        <v>26</v>
-      </c>
-      <c r="S1" s="19" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="2" spans="14:19" x14ac:dyDescent="0.25">
-      <c r="N2" s="14">
-        <v>0.762384490029694</v>
-      </c>
-      <c r="O2" s="15">
-        <v>0.44624975588118598</v>
-      </c>
-      <c r="P2" s="16">
-        <v>0.78551996118716705</v>
-      </c>
-      <c r="Q2" s="17">
-        <v>0.29160072506103601</v>
-      </c>
-      <c r="R2" s="18">
-        <v>0.82577386681059695</v>
-      </c>
-      <c r="S2" s="7">
-        <v>4.5710095337786E-2</v>
-      </c>
-    </row>
-    <row r="3" spans="14:19" x14ac:dyDescent="0.25">
-      <c r="N3" s="14">
-        <v>8.2901279432195593E-2</v>
-      </c>
-      <c r="O3" s="9">
-        <v>9.0782211164155292E-3</v>
-      </c>
-      <c r="P3" s="16">
-        <v>0.52024738694317496</v>
-      </c>
-      <c r="Q3" s="17">
-        <v>7.2269282640789106E-2</v>
-      </c>
-      <c r="R3" s="18">
-        <v>0.76388269721491497</v>
-      </c>
-      <c r="S3" s="19">
-        <v>0.45347930983877699</v>
-      </c>
-    </row>
-    <row r="4" spans="14:19" x14ac:dyDescent="0.25">
-      <c r="N4" s="14">
-        <v>6.6225124959576706E-2</v>
-      </c>
-      <c r="O4" s="15">
-        <v>0.61881514010194805</v>
-      </c>
-      <c r="P4" s="10">
-        <v>1.6347989883004101E-2</v>
-      </c>
-      <c r="Q4" s="11">
-        <v>1.1178235493982801E-2</v>
-      </c>
-      <c r="R4" s="18">
-        <v>0.41128551861353002</v>
-      </c>
-      <c r="S4" s="7">
-        <v>2.5966862137770701E-2</v>
-      </c>
-    </row>
-    <row r="5" spans="14:19" x14ac:dyDescent="0.25">
-      <c r="N5" s="14">
-        <v>0.33061324554751997</v>
-      </c>
-      <c r="O5" s="15">
-        <v>0.58761063110676703</v>
-      </c>
-      <c r="P5" s="16">
-        <v>0.876273721691745</v>
-      </c>
-      <c r="Q5" s="17">
-        <v>0.12610118972802201</v>
-      </c>
-      <c r="R5" s="18">
-        <v>0.84451617033304205</v>
-      </c>
-      <c r="S5" s="19">
-        <v>0.34787221257796602</v>
-      </c>
-    </row>
-    <row r="6" spans="14:19" x14ac:dyDescent="0.25">
-      <c r="N6" s="14">
-        <v>0.41886387925431101</v>
-      </c>
-      <c r="O6" s="15">
-        <v>0.54683519144140802</v>
-      </c>
-      <c r="P6" s="16">
-        <v>0.60936795919082498</v>
-      </c>
-      <c r="Q6" s="17">
-        <v>0.51888455220311103</v>
-      </c>
-      <c r="R6" s="18">
-        <v>0.92811381976317897</v>
-      </c>
-      <c r="S6" s="19">
-        <v>0.117144834533319</v>
-      </c>
-    </row>
-    <row r="7" spans="14:19" x14ac:dyDescent="0.25">
-      <c r="N7" s="14">
-        <v>0.73074475229926095</v>
-      </c>
-      <c r="O7" s="15">
-        <v>0.482119508817688</v>
-      </c>
-      <c r="P7" s="16">
-        <v>7.7299330333445299E-2</v>
-      </c>
-      <c r="Q7" s="17">
-        <v>0.41648763304756098</v>
-      </c>
-      <c r="R7" s="18">
-        <v>0.92618166088133702</v>
-      </c>
-      <c r="S7" s="7">
-        <v>1.5741522728162101E-2</v>
-      </c>
-    </row>
-    <row r="8" spans="14:19" x14ac:dyDescent="0.25">
-      <c r="N8" s="12">
-        <v>3.9736164584284001E-2</v>
-      </c>
-      <c r="O8" s="9">
-        <v>2.23753114222145E-3</v>
-      </c>
-      <c r="P8" s="10">
-        <v>2.4759724199063201E-3</v>
-      </c>
-      <c r="Q8" s="17">
-        <v>0.42442038054964198</v>
-      </c>
-      <c r="R8" s="18">
-        <v>0.57583799773840905</v>
-      </c>
-      <c r="S8" s="7">
-        <v>1.1238296525258799E-3</v>
-      </c>
-    </row>
-    <row r="9" spans="14:19" x14ac:dyDescent="0.25">
-      <c r="N9" s="14">
-        <v>0.30555896896170998</v>
-      </c>
-      <c r="O9" s="15">
-        <v>0.220796800536256</v>
-      </c>
-      <c r="P9" s="16">
-        <v>0.34273266373509897</v>
-      </c>
-      <c r="Q9" s="11">
-        <v>1.6849469393969401E-2</v>
-      </c>
-      <c r="R9" s="18">
-        <v>0.80207673397527102</v>
-      </c>
-      <c r="S9" s="19">
-        <v>8.3557084326203193E-2</v>
-      </c>
-    </row>
-    <row r="10" spans="14:19" x14ac:dyDescent="0.25">
-      <c r="N10" s="14">
-        <v>0.40967747091093998</v>
-      </c>
-      <c r="O10" s="9">
-        <v>4.93615335741312E-2</v>
-      </c>
-      <c r="P10" s="16">
-        <v>7.5060611423136706E-2</v>
-      </c>
-      <c r="Q10" s="17">
-        <v>5.3349459021998002E-2</v>
-      </c>
-      <c r="R10" s="18">
-        <v>0.83537027035042999</v>
-      </c>
-      <c r="S10" s="7">
-        <v>2.0751052693414899E-3</v>
-      </c>
-    </row>
-    <row r="11" spans="14:19" x14ac:dyDescent="0.25">
-      <c r="N11" s="14">
-        <v>0.312866167848105</v>
-      </c>
-      <c r="O11" s="15">
-        <v>0.36919882166698498</v>
-      </c>
-      <c r="P11" s="16">
-        <v>0.32044779172975002</v>
-      </c>
-      <c r="Q11" s="17">
-        <v>1.01926877470356</v>
-      </c>
-      <c r="R11" s="18">
-        <v>0.41730594570108798</v>
-      </c>
-      <c r="S11" s="19">
-        <v>0.32964773522541801</v>
-      </c>
-    </row>
-    <row r="12" spans="14:19" x14ac:dyDescent="0.25">
-      <c r="N12" s="14">
-        <v>0.673063017606508</v>
-      </c>
-      <c r="O12" s="15">
-        <v>0.48391674975244903</v>
-      </c>
-      <c r="P12" s="16">
-        <v>0.37967438937929698</v>
-      </c>
-      <c r="Q12" s="17">
-        <v>0.61551986182630103</v>
-      </c>
-      <c r="R12" s="18">
-        <v>0.96518223885221099</v>
-      </c>
-      <c r="S12" s="19">
-        <v>0.77989454444137896</v>
-      </c>
-    </row>
-    <row r="13" spans="14:19" x14ac:dyDescent="0.25">
-      <c r="N13" s="14">
-        <v>9.5712795892028399E-2</v>
-      </c>
-      <c r="O13" s="15">
-        <v>0.44634237725270698</v>
-      </c>
-      <c r="P13" s="16">
-        <v>0.31255665386579601</v>
-      </c>
-      <c r="Q13" s="17">
-        <v>0.98678976939878205</v>
-      </c>
-      <c r="R13" s="18">
-        <v>0.517815470814041</v>
-      </c>
-      <c r="S13" s="19">
-        <v>0.297478016852251</v>
-      </c>
-    </row>
-    <row r="14" spans="14:19" x14ac:dyDescent="0.25">
-      <c r="N14" s="14">
-        <v>0.174295602147962</v>
-      </c>
-      <c r="O14" s="15">
-        <v>0.86844583111990603</v>
-      </c>
-      <c r="P14" s="10">
-        <v>4.3268390080787603E-2</v>
-      </c>
-      <c r="Q14" s="11">
-        <v>8.3521584494051695E-3</v>
-      </c>
-      <c r="R14" s="18">
-        <v>0.81524617305381997</v>
-      </c>
-      <c r="S14" s="19">
-        <v>6.5292475138674894E-2</v>
-      </c>
-    </row>
-    <row r="15" spans="14:19" x14ac:dyDescent="0.25">
-      <c r="N15" s="12">
-        <v>4.0424970068182499E-3</v>
-      </c>
-      <c r="O15" s="15">
-        <v>5.7965913592618802E-2</v>
-      </c>
-      <c r="P15" s="16">
-        <v>0.218104991549528</v>
-      </c>
-      <c r="Q15" s="11">
-        <v>1.17388410353965E-2</v>
-      </c>
-      <c r="R15" s="18">
-        <v>0.21974386864794401</v>
-      </c>
-      <c r="S15" s="19">
-        <v>0.26584607245743602</v>
-      </c>
-    </row>
-    <row r="16" spans="14:19" x14ac:dyDescent="0.25">
-      <c r="N16" s="12">
-        <v>8.8957362296602296E-3</v>
-      </c>
-      <c r="O16" s="15">
-        <v>0.31603437363464698</v>
-      </c>
-      <c r="P16" s="16">
-        <v>0.250267714639267</v>
-      </c>
-      <c r="Q16" s="17">
-        <v>1.01343777505961</v>
-      </c>
-      <c r="R16" s="18">
-        <v>0.88243598341370999</v>
-      </c>
-      <c r="S16" s="19">
-        <v>0.45617091532496501</v>
+        <v>1.4760844231147061</v>
       </c>
     </row>
   </sheetData>
@@ -33428,332 +34256,1118 @@
 
 <file path=xl/worksheets/sheet36.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="N1:S16"/>
+  <dimension ref="A1:M38"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="N1" sqref="N1:S16"/>
+      <selection activeCell="A38" sqref="A38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="14:19" x14ac:dyDescent="0.25">
-      <c r="N1" s="14" t="s">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="O1" s="15" t="s">
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="P1" s="16" t="s">
+      <c r="F1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="Q1" s="17" t="s">
+      <c r="H1" t="s">
+        <v>4</v>
+      </c>
+      <c r="I1" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="R1" s="18" t="s">
+      <c r="J1" t="s">
+        <v>5</v>
+      </c>
+      <c r="K1" s="18" t="s">
         <v>26</v>
       </c>
-      <c r="S1" s="19" t="s">
+      <c r="L1" t="s">
+        <v>6</v>
+      </c>
+      <c r="M1" s="19" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="2" spans="14:19" x14ac:dyDescent="0.25">
-      <c r="N2" s="14">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2">
+        <v>0.44325947225759649</v>
+      </c>
+      <c r="C2" s="14">
         <v>0.762384490029694</v>
       </c>
-      <c r="O2" s="15">
+      <c r="D2">
+        <v>0.13268020637699676</v>
+      </c>
+      <c r="E2" s="15">
         <v>0.44624975588118598</v>
       </c>
-      <c r="P2" s="16">
+      <c r="F2">
+        <v>1.3596341086186523</v>
+      </c>
+      <c r="G2" s="16">
         <v>0.78551996118716705</v>
       </c>
-      <c r="Q2" s="17">
+      <c r="H2">
+        <v>0.124008318768719</v>
+      </c>
+      <c r="I2" s="17">
         <v>0.29160072506103601</v>
       </c>
-      <c r="R2" s="18">
+      <c r="J2">
+        <v>0.19964830210412457</v>
+      </c>
+      <c r="K2" s="18">
         <v>0.82577386681059695</v>
       </c>
-      <c r="S2" s="7">
+      <c r="L2">
+        <v>1.1875522213411989</v>
+      </c>
+      <c r="M2" s="7">
         <v>4.5710095337786E-2</v>
       </c>
     </row>
-    <row r="3" spans="14:19" x14ac:dyDescent="0.25">
-      <c r="N3" s="14">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3">
+        <v>0.35721726153263667</v>
+      </c>
+      <c r="C3" s="14">
         <v>8.2901279432195593E-2</v>
       </c>
-      <c r="O3" s="9">
+      <c r="D3">
+        <v>1.0517467736638961</v>
+      </c>
+      <c r="E3" s="9">
         <v>9.0782211164155292E-3</v>
       </c>
-      <c r="P3" s="16">
+      <c r="F3">
+        <v>0.50786706273900151</v>
+      </c>
+      <c r="G3" s="16">
         <v>0.52024738694317496</v>
       </c>
-      <c r="Q3" s="17">
+      <c r="H3">
+        <v>0.45751694034791596</v>
+      </c>
+      <c r="I3" s="17">
         <v>7.2269282640789106E-2</v>
       </c>
-      <c r="R3" s="18">
+      <c r="J3">
+        <v>1.2413307934798183</v>
+      </c>
+      <c r="K3" s="18">
         <v>0.76388269721491497</v>
       </c>
-      <c r="S3" s="19">
+      <c r="L3">
+        <v>1.427532538740345</v>
+      </c>
+      <c r="M3" s="19">
         <v>0.45347930983877699</v>
       </c>
     </row>
-    <row r="4" spans="14:19" x14ac:dyDescent="0.25">
-      <c r="N4" s="14">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4">
+        <v>0.72086927135374101</v>
+      </c>
+      <c r="C4" s="14">
         <v>6.6225124959576706E-2</v>
       </c>
-      <c r="O4" s="15">
+      <c r="D4">
+        <v>0.14496421249999999</v>
+      </c>
+      <c r="E4" s="15">
         <v>0.61881514010194805</v>
       </c>
-      <c r="P4" s="10">
+      <c r="F4">
+        <v>0.83475365197106821</v>
+      </c>
+      <c r="G4" s="10">
         <v>1.6347989883004101E-2</v>
       </c>
-      <c r="Q4" s="11">
+      <c r="H4">
+        <v>1.1317583924195833</v>
+      </c>
+      <c r="I4" s="11">
         <v>1.1178235493982801E-2</v>
       </c>
-      <c r="R4" s="18">
+      <c r="J4">
+        <v>1.1051102056902664</v>
+      </c>
+      <c r="K4" s="18">
         <v>0.41128551861353002</v>
       </c>
-      <c r="S4" s="7">
+      <c r="L4">
+        <v>0.84035969615263495</v>
+      </c>
+      <c r="M4" s="7">
         <v>2.5966862137770701E-2</v>
       </c>
     </row>
-    <row r="5" spans="14:19" x14ac:dyDescent="0.25">
-      <c r="N5" s="14">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5">
+        <v>0.47595022871536047</v>
+      </c>
+      <c r="C5" s="14">
         <v>0.33061324554751997</v>
       </c>
-      <c r="O5" s="15">
+      <c r="D5">
+        <v>0.55050345591266892</v>
+      </c>
+      <c r="E5" s="15">
         <v>0.58761063110676703</v>
       </c>
-      <c r="P5" s="16">
+      <c r="F5">
+        <v>0.77109217217433546</v>
+      </c>
+      <c r="G5" s="16">
         <v>0.876273721691745</v>
       </c>
-      <c r="Q5" s="17">
+      <c r="H5">
+        <v>0.84337951581849058</v>
+      </c>
+      <c r="I5" s="17">
         <v>0.12610118972802201</v>
       </c>
-      <c r="R5" s="18">
+      <c r="J5">
+        <v>0.5599627871173336</v>
+      </c>
+      <c r="K5" s="18">
         <v>0.84451617033304205</v>
       </c>
-      <c r="S5" s="19">
+      <c r="L5">
+        <v>0.21970417308426202</v>
+      </c>
+      <c r="M5" s="19">
         <v>0.34787221257796602</v>
       </c>
     </row>
-    <row r="6" spans="14:19" x14ac:dyDescent="0.25">
-      <c r="N6" s="14">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6">
+        <v>0.45479844133053099</v>
+      </c>
+      <c r="C6" s="14">
         <v>0.41886387925431101</v>
       </c>
-      <c r="O6" s="15">
+      <c r="D6">
+        <v>0.17380139994281638</v>
+      </c>
+      <c r="E6" s="15">
         <v>0.54683519144140802</v>
       </c>
-      <c r="P6" s="16">
+      <c r="F6">
+        <v>0.35326105333333335</v>
+      </c>
+      <c r="G6" s="16">
         <v>0.60936795919082498</v>
       </c>
-      <c r="Q6" s="17">
+      <c r="H6">
+        <v>0.21916875916366999</v>
+      </c>
+      <c r="I6" s="17">
         <v>0.51888455220311103</v>
       </c>
-      <c r="R6" s="18">
+      <c r="J6">
+        <v>0.24178273806551065</v>
+      </c>
+      <c r="K6" s="18">
         <v>0.92811381976317897</v>
       </c>
-      <c r="S6" s="19">
+      <c r="L6">
+        <v>0.13430588664337054</v>
+      </c>
+      <c r="M6" s="19">
         <v>0.117144834533319</v>
       </c>
     </row>
-    <row r="7" spans="14:19" x14ac:dyDescent="0.25">
-      <c r="N7" s="14">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7">
+        <v>1.9405029647740497</v>
+      </c>
+      <c r="C7" s="14">
         <v>0.73074475229926095</v>
       </c>
-      <c r="O7" s="15">
+      <c r="D7">
+        <v>1.4075136988561026</v>
+      </c>
+      <c r="E7" s="15">
         <v>0.482119508817688</v>
       </c>
-      <c r="P7" s="16">
+      <c r="F7">
+        <v>1.8636293352242859</v>
+      </c>
+      <c r="G7" s="16">
         <v>7.7299330333445299E-2</v>
       </c>
-      <c r="Q7" s="17">
+      <c r="H7">
+        <v>0.4916199175</v>
+      </c>
+      <c r="I7" s="17">
         <v>0.41648763304756098</v>
       </c>
-      <c r="R7" s="18">
+      <c r="J7">
+        <v>1.628290996381083</v>
+      </c>
+      <c r="K7" s="18">
         <v>0.92618166088133702</v>
       </c>
-      <c r="S7" s="7">
+      <c r="L7">
+        <v>0.53352945472475433</v>
+      </c>
+      <c r="M7" s="7">
         <v>1.5741522728162101E-2</v>
       </c>
     </row>
-    <row r="8" spans="14:19" x14ac:dyDescent="0.25">
-      <c r="N8" s="12">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8">
+        <v>0.62834130637483843</v>
+      </c>
+      <c r="C8" s="12">
         <v>3.9736164584284001E-2</v>
       </c>
-      <c r="O8" s="9">
+      <c r="D8">
+        <v>0.73381235939887679</v>
+      </c>
+      <c r="E8" s="9">
         <v>2.23753114222145E-3</v>
       </c>
-      <c r="P8" s="10">
+      <c r="F8">
+        <v>0.310928262790445</v>
+      </c>
+      <c r="G8" s="10">
         <v>2.4759724199063201E-3</v>
       </c>
-      <c r="Q8" s="17">
+      <c r="H8">
+        <v>2.7819706069563099</v>
+      </c>
+      <c r="I8" s="17">
         <v>0.42442038054964198</v>
       </c>
-      <c r="R8" s="18">
+      <c r="J8">
+        <v>0.5935956166666666</v>
+      </c>
+      <c r="K8" s="18">
         <v>0.57583799773840905</v>
       </c>
-      <c r="S8" s="7">
+      <c r="L8">
+        <v>0.54519033347722201</v>
+      </c>
+      <c r="M8" s="7">
         <v>1.1238296525258799E-3</v>
       </c>
     </row>
-    <row r="9" spans="14:19" x14ac:dyDescent="0.25">
-      <c r="N9" s="14">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>14</v>
+      </c>
+      <c r="B9">
+        <v>0.5151313497252461</v>
+      </c>
+      <c r="C9" s="14">
         <v>0.30555896896170998</v>
       </c>
-      <c r="O9" s="15">
+      <c r="D9">
+        <v>0.29691249909334511</v>
+      </c>
+      <c r="E9" s="15">
         <v>0.220796800536256</v>
       </c>
-      <c r="P9" s="16">
+      <c r="F9">
+        <v>0.85066868055168232</v>
+      </c>
+      <c r="G9" s="16">
         <v>0.34273266373509897</v>
       </c>
-      <c r="Q9" s="11">
+      <c r="H9">
+        <v>0.25855186403289848</v>
+      </c>
+      <c r="I9" s="11">
         <v>1.6849469393969401E-2</v>
       </c>
-      <c r="R9" s="18">
+      <c r="J9">
+        <v>0.57416629219765281</v>
+      </c>
+      <c r="K9" s="18">
         <v>0.80207673397527102</v>
       </c>
-      <c r="S9" s="19">
+      <c r="L9">
+        <v>0.27663869537363994</v>
+      </c>
+      <c r="M9" s="19">
         <v>8.3557084326203193E-2</v>
       </c>
     </row>
-    <row r="10" spans="14:19" x14ac:dyDescent="0.25">
-      <c r="N10" s="14">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>15</v>
+      </c>
+      <c r="B10">
+        <v>0.99285189498340465</v>
+      </c>
+      <c r="C10" s="14">
         <v>0.40967747091093998</v>
       </c>
-      <c r="O10" s="9">
+      <c r="D10">
+        <v>0.27431542900946598</v>
+      </c>
+      <c r="E10" s="9">
         <v>4.93615335741312E-2</v>
       </c>
-      <c r="P10" s="16">
+      <c r="F10">
+        <v>0.95166223244277104</v>
+      </c>
+      <c r="G10" s="16">
         <v>7.5060611423136706E-2</v>
       </c>
-      <c r="Q10" s="17">
+      <c r="H10">
+        <v>0.19061430953629951</v>
+      </c>
+      <c r="I10" s="17">
         <v>5.3349459021998002E-2</v>
       </c>
-      <c r="R10" s="18">
+      <c r="J10">
+        <v>1.1848382874958401</v>
+      </c>
+      <c r="K10" s="18">
         <v>0.83537027035042999</v>
       </c>
-      <c r="S10" s="7">
+      <c r="L10">
+        <v>0.3051527242353182</v>
+      </c>
+      <c r="M10" s="7">
         <v>2.0751052693414899E-3</v>
       </c>
     </row>
-    <row r="11" spans="14:19" x14ac:dyDescent="0.25">
-      <c r="N11" s="14">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>16</v>
+      </c>
+      <c r="B11">
+        <v>2.0731109833820467</v>
+      </c>
+      <c r="C11" s="14">
         <v>0.312866167848105</v>
       </c>
-      <c r="O11" s="15">
+      <c r="D11">
+        <v>1.0089956841730834</v>
+      </c>
+      <c r="E11" s="15">
         <v>0.36919882166698498</v>
       </c>
-      <c r="P11" s="16">
+      <c r="F11">
+        <v>0.27109189654249871</v>
+      </c>
+      <c r="G11" s="16">
         <v>0.32044779172975002</v>
       </c>
-      <c r="Q11" s="17">
+      <c r="H11">
+        <v>0.14031764784486581</v>
+      </c>
+      <c r="I11" s="17">
         <v>1.01926877470356</v>
       </c>
-      <c r="R11" s="18">
+      <c r="J11">
+        <v>0.65524707464767207</v>
+      </c>
+      <c r="K11" s="18">
         <v>0.41730594570108798</v>
       </c>
-      <c r="S11" s="19">
+      <c r="L11">
+        <v>1.2720413499065832</v>
+      </c>
+      <c r="M11" s="19">
         <v>0.32964773522541801</v>
       </c>
     </row>
-    <row r="12" spans="14:19" x14ac:dyDescent="0.25">
-      <c r="N12" s="14">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>17</v>
+      </c>
+      <c r="B12">
+        <v>0.29069202061582444</v>
+      </c>
+      <c r="C12" s="14">
         <v>0.673063017606508</v>
       </c>
-      <c r="O12" s="15">
+      <c r="D12">
+        <v>0.60900463060432808</v>
+      </c>
+      <c r="E12" s="15">
         <v>0.48391674975244903</v>
       </c>
-      <c r="P12" s="16">
+      <c r="F12">
+        <v>0.45273866545323399</v>
+      </c>
+      <c r="G12" s="16">
         <v>0.37967438937929698</v>
       </c>
-      <c r="Q12" s="17">
+      <c r="H12">
+        <v>0.21213043851485261</v>
+      </c>
+      <c r="I12" s="17">
         <v>0.61551986182630103</v>
       </c>
-      <c r="R12" s="18">
+      <c r="J12">
+        <v>0.31908102381470055</v>
+      </c>
+      <c r="K12" s="18">
         <v>0.96518223885221099</v>
       </c>
-      <c r="S12" s="19">
+      <c r="L12">
+        <v>0.24787793816426176</v>
+      </c>
+      <c r="M12" s="19">
         <v>0.77989454444137896</v>
       </c>
     </row>
-    <row r="13" spans="14:19" x14ac:dyDescent="0.25">
-      <c r="N13" s="14">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>18</v>
+      </c>
+      <c r="B13">
+        <v>0.45165798193351342</v>
+      </c>
+      <c r="C13" s="14">
         <v>9.5712795892028399E-2</v>
       </c>
-      <c r="O13" s="15">
+      <c r="D13">
+        <v>0.23819370307047871</v>
+      </c>
+      <c r="E13" s="15">
         <v>0.44634237725270698</v>
       </c>
-      <c r="P13" s="16">
+      <c r="F13">
+        <v>0.29029346182852955</v>
+      </c>
+      <c r="G13" s="16">
         <v>0.31255665386579601</v>
       </c>
-      <c r="Q13" s="17">
+      <c r="H13">
+        <v>0.54992711132400174</v>
+      </c>
+      <c r="I13" s="17">
         <v>0.98678976939878205</v>
       </c>
-      <c r="R13" s="18">
+      <c r="J13">
+        <v>0.2944452164443585</v>
+      </c>
+      <c r="K13" s="18">
         <v>0.517815470814041</v>
       </c>
-      <c r="S13" s="19">
+      <c r="L13">
+        <v>0.24418910898710591</v>
+      </c>
+      <c r="M13" s="19">
         <v>0.297478016852251</v>
       </c>
     </row>
-    <row r="14" spans="14:19" x14ac:dyDescent="0.25">
-      <c r="N14" s="14">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>19</v>
+      </c>
+      <c r="B14">
+        <v>0.67914781305819294</v>
+      </c>
+      <c r="C14" s="14">
         <v>0.174295602147962</v>
       </c>
-      <c r="O14" s="15">
+      <c r="D14">
+        <v>0.70667901535708821</v>
+      </c>
+      <c r="E14" s="15">
         <v>0.86844583111990603</v>
       </c>
-      <c r="P14" s="10">
+      <c r="F14">
+        <v>1.137913966938201</v>
+      </c>
+      <c r="G14" s="10">
         <v>4.3268390080787603E-2</v>
       </c>
-      <c r="Q14" s="11">
+      <c r="H14">
+        <v>0.30057566966756066</v>
+      </c>
+      <c r="I14" s="11">
         <v>8.3521584494051695E-3</v>
       </c>
-      <c r="R14" s="18">
+      <c r="J14">
+        <v>0.39455644122463873</v>
+      </c>
+      <c r="K14" s="18">
         <v>0.81524617305381997</v>
       </c>
-      <c r="S14" s="19">
+      <c r="L14">
+        <v>0.46350032464944985</v>
+      </c>
+      <c r="M14" s="19">
         <v>6.5292475138674894E-2</v>
       </c>
     </row>
-    <row r="15" spans="14:19" x14ac:dyDescent="0.25">
-      <c r="N15" s="12">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>20</v>
+      </c>
+      <c r="B15">
+        <v>0.38876244658913434</v>
+      </c>
+      <c r="C15" s="12">
         <v>4.0424970068182499E-3</v>
       </c>
-      <c r="O15" s="15">
+      <c r="D15">
+        <v>0.77623919848867418</v>
+      </c>
+      <c r="E15" s="15">
         <v>5.7965913592618802E-2</v>
       </c>
-      <c r="P15" s="16">
+      <c r="F15">
+        <v>1.6560246615692416</v>
+      </c>
+      <c r="G15" s="16">
         <v>0.218104991549528</v>
       </c>
-      <c r="Q15" s="11">
+      <c r="H15">
+        <v>0.62044886302659485</v>
+      </c>
+      <c r="I15" s="11">
         <v>1.17388410353965E-2</v>
       </c>
-      <c r="R15" s="18">
+      <c r="J15">
+        <v>0.78861663136541316</v>
+      </c>
+      <c r="K15" s="18">
         <v>0.21974386864794401</v>
       </c>
-      <c r="S15" s="19">
+      <c r="L15">
+        <v>0.45333405866781645</v>
+      </c>
+      <c r="M15" s="19">
         <v>0.26584607245743602</v>
       </c>
     </row>
-    <row r="16" spans="14:19" x14ac:dyDescent="0.25">
-      <c r="N16" s="12">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>21</v>
+      </c>
+      <c r="B16">
+        <v>2.3016728479461759</v>
+      </c>
+      <c r="C16" s="12">
         <v>8.8957362296602296E-3</v>
       </c>
-      <c r="O16" s="15">
+      <c r="D16">
+        <v>0.6802428223504221</v>
+      </c>
+      <c r="E16" s="15">
         <v>0.31603437363464698</v>
       </c>
-      <c r="P16" s="16">
+      <c r="F16">
+        <v>1.2797739428045249</v>
+      </c>
+      <c r="G16" s="16">
         <v>0.250267714639267</v>
       </c>
-      <c r="Q16" s="17">
+      <c r="H16">
+        <v>1.1258438911699027</v>
+      </c>
+      <c r="I16" s="17">
         <v>1.01343777505961</v>
       </c>
-      <c r="R16" s="18">
+      <c r="J16">
+        <v>0.45434464473058628</v>
+      </c>
+      <c r="K16" s="18">
         <v>0.88243598341370999</v>
       </c>
-      <c r="S16" s="19">
+      <c r="L16">
+        <v>3.1590337508333337</v>
+      </c>
+      <c r="M16" s="19">
         <v>0.45617091532496501</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>7</v>
+      </c>
+      <c r="B21">
+        <f>B2-dhap4!B2</f>
+        <v>2.8864768460611145E-2</v>
+      </c>
+      <c r="D21">
+        <f>D2-dhap4!D2</f>
+        <v>3.6598539195904584E-2</v>
+      </c>
+      <c r="F21">
+        <f>F2-dhap4!F2</f>
+        <v>5.3592846037092912E-2</v>
+      </c>
+      <c r="H21">
+        <f>H2-dhap4!H2</f>
+        <v>-2.1955928803476424E-2</v>
+      </c>
+      <c r="J21">
+        <f>J2-dhap4!J2</f>
+        <v>-1.0959375100483226E-2</v>
+      </c>
+      <c r="L21">
+        <f>L2-dhap4!L2</f>
+        <v>0.3405942454896258</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>8</v>
+      </c>
+      <c r="B22">
+        <f>B3-dhap4!B3</f>
+        <v>0.10362699796979885</v>
+      </c>
+      <c r="D22">
+        <f>D3-dhap4!D3</f>
+        <v>0.75137720420804666</v>
+      </c>
+      <c r="F22">
+        <f>F3-dhap4!F3</f>
+        <v>-0.12640634204988088</v>
+      </c>
+      <c r="H22">
+        <f>H3-dhap4!H3</f>
+        <v>0.14131888028341233</v>
+      </c>
+      <c r="J22">
+        <f>J3-dhap4!J3</f>
+        <v>4.8019749002692125E-2</v>
+      </c>
+      <c r="L22">
+        <f>L3-dhap4!L3</f>
+        <v>0.23248410925299945</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>9</v>
+      </c>
+      <c r="B23">
+        <f>B4-dhap4!B4</f>
+        <v>-0.10855556974830716</v>
+      </c>
+      <c r="D23">
+        <f>D4-dhap4!D4</f>
+        <v>0</v>
+      </c>
+      <c r="F23">
+        <f>F4-dhap4!F4</f>
+        <v>-3.3166406703207252E-2</v>
+      </c>
+      <c r="H23">
+        <f>H4-dhap4!H4</f>
+        <v>3.7406068842416929E-2</v>
+      </c>
+      <c r="J23">
+        <f>J4-dhap4!J4</f>
+        <v>0.33539504171145762</v>
+      </c>
+      <c r="L23">
+        <f>L4-dhap4!L4</f>
+        <v>0.16289681491083796</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>10</v>
+      </c>
+      <c r="B24">
+        <f>B5-dhap4!B5</f>
+        <v>-3.6077099159846082E-2</v>
+      </c>
+      <c r="D24">
+        <f>D5-dhap4!D5</f>
+        <v>-0.35342218814062809</v>
+      </c>
+      <c r="F24">
+        <f>F5-dhap4!F5</f>
+        <v>1.9148907914063873E-3</v>
+      </c>
+      <c r="H24">
+        <f>H5-dhap4!H5</f>
+        <v>-4.2348203373860027E-2</v>
+      </c>
+      <c r="J24">
+        <f>J5-dhap4!J5</f>
+        <v>5.6674963019809455E-2</v>
+      </c>
+      <c r="L24">
+        <f>L5-dhap4!L5</f>
+        <v>-8.9998495505981824E-3</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>11</v>
+      </c>
+      <c r="B25">
+        <f>B6-dhap4!B6</f>
+        <v>-1.9529110246622239E-2</v>
+      </c>
+      <c r="D25">
+        <f>D6-dhap4!D6</f>
+        <v>-2.7596917499196155E-2</v>
+      </c>
+      <c r="F25">
+        <f>F6-dhap4!F6</f>
+        <v>0</v>
+      </c>
+      <c r="H25">
+        <f>H6-dhap4!H6</f>
+        <v>3.2409526046149106E-2</v>
+      </c>
+      <c r="J25">
+        <f>J6-dhap4!J6</f>
+        <v>4.7359279700975865E-3</v>
+      </c>
+      <c r="L25">
+        <f>L6-dhap4!L6</f>
+        <v>-3.7915139803549602E-2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>12</v>
+      </c>
+      <c r="B26">
+        <f>B7-dhap4!B7</f>
+        <v>-0.20961370757679743</v>
+      </c>
+      <c r="D26">
+        <f>D7-dhap4!D7</f>
+        <v>0.24648571415261822</v>
+      </c>
+      <c r="F26">
+        <f>F7-dhap4!F7</f>
+        <v>0.51903390250431158</v>
+      </c>
+      <c r="H26">
+        <f>H7-dhap4!H7</f>
+        <v>0</v>
+      </c>
+      <c r="J26">
+        <f>J7-dhap4!J7</f>
+        <v>0.2069047546963847</v>
+      </c>
+      <c r="L26">
+        <f>L7-dhap4!L7</f>
+        <v>-2.6140624261137724E-2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>13</v>
+      </c>
+      <c r="B27">
+        <f>B8-dhap4!B8</f>
+        <v>1.060000732175348E-2</v>
+      </c>
+      <c r="D27">
+        <f>D8-dhap4!D8</f>
+        <v>4.9756967375260253E-2</v>
+      </c>
+      <c r="F27">
+        <f>F8-dhap4!F8</f>
+        <v>1.4209147748203033E-2</v>
+      </c>
+      <c r="H27">
+        <f>H8-dhap4!H8</f>
+        <v>-4.5664676302267893E-2</v>
+      </c>
+      <c r="J27">
+        <f>J8-dhap4!J8</f>
+        <v>0</v>
+      </c>
+      <c r="L27">
+        <f>L8-dhap4!L8</f>
+        <v>2.1273161402035168E-2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>14</v>
+      </c>
+      <c r="B28">
+        <f>B9-dhap4!B9</f>
+        <v>5.166020286617462E-2</v>
+      </c>
+      <c r="D28">
+        <f>D9-dhap4!D9</f>
+        <v>-8.7754378366363017E-2</v>
+      </c>
+      <c r="F28">
+        <f>F9-dhap4!F9</f>
+        <v>8.1363840725335979E-2</v>
+      </c>
+      <c r="H28">
+        <f>H9-dhap4!H9</f>
+        <v>5.16407960853425E-2</v>
+      </c>
+      <c r="J28">
+        <f>J9-dhap4!J9</f>
+        <v>0.12514975027752945</v>
+      </c>
+      <c r="L28">
+        <f>L9-dhap4!L9</f>
+        <v>2.667594668583792E-2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>15</v>
+      </c>
+      <c r="B29">
+        <f>B10-dhap4!B10</f>
+        <v>1.0373011562460288E-2</v>
+      </c>
+      <c r="D29">
+        <f>D10-dhap4!D10</f>
+        <v>-3.1305141154894245E-2</v>
+      </c>
+      <c r="F29">
+        <f>F10-dhap4!F10</f>
+        <v>-1.8959326543184329E-2</v>
+      </c>
+      <c r="H29">
+        <f>H10-dhap4!H10</f>
+        <v>1.2427188647950421E-2</v>
+      </c>
+      <c r="J29">
+        <f>J10-dhap4!J10</f>
+        <v>-8.4836329317350412E-4</v>
+      </c>
+      <c r="L29">
+        <f>L10-dhap4!L10</f>
+        <v>3.5395821104895808E-2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>16</v>
+      </c>
+      <c r="B30">
+        <f>B11-dhap4!B11</f>
+        <v>0.27676360279959411</v>
+      </c>
+      <c r="D30">
+        <f>D11-dhap4!D11</f>
+        <v>0.1328655132990838</v>
+      </c>
+      <c r="F30">
+        <f>F11-dhap4!F11</f>
+        <v>-0.1179106061424266</v>
+      </c>
+      <c r="H30">
+        <f>H11-dhap4!H11</f>
+        <v>-3.3660899733663319E-2</v>
+      </c>
+      <c r="J30">
+        <f>J11-dhap4!J11</f>
+        <v>0.12149772142571913</v>
+      </c>
+      <c r="L30">
+        <f>L11-dhap4!L11</f>
+        <v>-7.5408568586554647E-2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>17</v>
+      </c>
+      <c r="B31">
+        <f>B12-dhap4!B12</f>
+        <v>-1.832550968215696E-2</v>
+      </c>
+      <c r="D31">
+        <f>D12-dhap4!D12</f>
+        <v>-8.9548882235882643E-2</v>
+      </c>
+      <c r="F31">
+        <f>F12-dhap4!F12</f>
+        <v>-1.6902296548972906E-2</v>
+      </c>
+      <c r="H31">
+        <f>H12-dhap4!H12</f>
+        <v>2.101236175259602E-2</v>
+      </c>
+      <c r="J31">
+        <f>J12-dhap4!J12</f>
+        <v>-1.0195089393501E-3</v>
+      </c>
+      <c r="L31">
+        <f>L12-dhap4!L12</f>
+        <v>1.5740345615503637E-3</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>18</v>
+      </c>
+      <c r="B32">
+        <f>B13-dhap4!B13</f>
+        <v>4.8067081792505906E-2</v>
+      </c>
+      <c r="D32">
+        <f>D13-dhap4!D13</f>
+        <v>1.1991561379513432E-2</v>
+      </c>
+      <c r="F32">
+        <f>F13-dhap4!F13</f>
+        <v>1.0079494779811349E-2</v>
+      </c>
+      <c r="H32">
+        <f>H13-dhap4!H13</f>
+        <v>8.5437000036076571E-2</v>
+      </c>
+      <c r="J32">
+        <f>J13-dhap4!J13</f>
+        <v>5.3440233190597652E-2</v>
+      </c>
+      <c r="L32">
+        <f>L13-dhap4!L13</f>
+        <v>-7.0288531714136487E-2</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>19</v>
+      </c>
+      <c r="B33">
+        <f>B14-dhap4!B14</f>
+        <v>-5.4907552564090412E-2</v>
+      </c>
+      <c r="D33">
+        <f>D14-dhap4!D14</f>
+        <v>8.2940912006989609E-2</v>
+      </c>
+      <c r="F33">
+        <f>F14-dhap4!F14</f>
+        <v>9.5528803407808782E-2</v>
+      </c>
+      <c r="H33">
+        <f>H14-dhap4!H14</f>
+        <v>4.7032254792028771E-2</v>
+      </c>
+      <c r="J33">
+        <f>J14-dhap4!J14</f>
+        <v>0.10775636677747674</v>
+      </c>
+      <c r="L33">
+        <f>L14-dhap4!L14</f>
+        <v>-6.3902406107730403E-2</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>20</v>
+      </c>
+      <c r="B34">
+        <f>B15-dhap4!B15</f>
+        <v>-1.6141193267677545E-2</v>
+      </c>
+      <c r="D34">
+        <f>D15-dhap4!D15</f>
+        <v>4.232520543783902E-2</v>
+      </c>
+      <c r="F34">
+        <f>F15-dhap4!F15</f>
+        <v>0.1671042356173158</v>
+      </c>
+      <c r="H34">
+        <f>H15-dhap4!H15</f>
+        <v>-0.10340857757571165</v>
+      </c>
+      <c r="J34">
+        <f>J15-dhap4!J15</f>
+        <v>0.12772457433945938</v>
+      </c>
+      <c r="L34">
+        <f>L15-dhap4!L15</f>
+        <v>-5.0646367333188891E-2</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>21</v>
+      </c>
+      <c r="B35">
+        <f>B16-dhap4!B16</f>
+        <v>-2.0668372790799694E-3</v>
+      </c>
+      <c r="D35">
+        <f>D16-dhap4!D16</f>
+        <v>6.7844876008748001E-3</v>
+      </c>
+      <c r="F35">
+        <f>F16-dhap4!F16</f>
+        <v>-4.4592949995170272E-4</v>
+      </c>
+      <c r="H35">
+        <f>H16-dhap4!H16</f>
+        <v>-2.9267186036312509E-3</v>
+      </c>
+      <c r="J35">
+        <f>J16-dhap4!J16</f>
+        <v>-6.5124918133162568E-3</v>
+      </c>
+      <c r="L35">
+        <f>L16-dhap4!L16</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <v>1.5009483703776725</v>
       </c>
     </row>
   </sheetData>
@@ -34483,8 +36097,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:W33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
-      <selection activeCell="W9" sqref="W9"/>
+    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
+      <selection activeCell="AL6" sqref="AL6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -35587,6 +37201,9 @@
       <c r="U32" t="s">
         <v>166</v>
       </c>
+      <c r="V32">
+        <v>1.4760844231147061</v>
+      </c>
       <c r="W32">
         <v>1.42628994475691</v>
       </c>
@@ -35595,12 +37212,21 @@
       <c r="U33" t="s">
         <v>173</v>
       </c>
+      <c r="V33">
+        <v>1.5009483703776725</v>
+      </c>
       <c r="W33">
         <v>1.42628994475691</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="N7:S7"/>
+    <mergeCell ref="N2:S2"/>
+    <mergeCell ref="N3:S3"/>
+    <mergeCell ref="N4:S4"/>
+    <mergeCell ref="N5:S5"/>
+    <mergeCell ref="N6:S6"/>
     <mergeCell ref="N14:S14"/>
     <mergeCell ref="N15:S15"/>
     <mergeCell ref="N16:S16"/>
@@ -35610,12 +37236,6 @@
     <mergeCell ref="N11:S11"/>
     <mergeCell ref="N12:S12"/>
     <mergeCell ref="N13:S13"/>
-    <mergeCell ref="N7:S7"/>
-    <mergeCell ref="N2:S2"/>
-    <mergeCell ref="N3:S3"/>
-    <mergeCell ref="N4:S4"/>
-    <mergeCell ref="N5:S5"/>
-    <mergeCell ref="N6:S6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>